<commit_message>
nyicil revisi postal error
</commit_message>
<xml_diff>
--- a/postal_error.xlsx
+++ b/postal_error.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="528">
   <si>
     <t>MYRKETAPANG</t>
   </si>
@@ -1595,6 +1595,9 @@
   </si>
   <si>
     <t>REVISION</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -2059,23 +2062,21 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
+      <right style="thin">
         <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </right>
-      <top/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -2124,14 +2125,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2177,13 +2177,37 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -2352,21 +2376,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J294" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J294" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A1:J294">
     <filterColumn colId="9"/>
   </autoFilter>
   <tableColumns count="10">
     <tableColumn id="1" name="ROW"/>
     <tableColumn id="2" name="COMPANY REFERENCE"/>
-    <tableColumn id="3" name="LOCATION" dataDxfId="6"/>
-    <tableColumn id="4" name="ADDRESS 1" dataDxfId="5"/>
-    <tableColumn id="5" name="ADDRESS 2" dataDxfId="4"/>
-    <tableColumn id="6" name="ADDRESS 3" dataDxfId="3"/>
-    <tableColumn id="7" name="LATITUDE" dataDxfId="2"/>
-    <tableColumn id="8" name="LONGITUDE" dataDxfId="1"/>
-    <tableColumn id="9" name="POSTAL CODE" dataDxfId="0"/>
-    <tableColumn id="10" name="REVISION"/>
+    <tableColumn id="3" name="LOCATION" dataDxfId="7"/>
+    <tableColumn id="4" name="ADDRESS 1" dataDxfId="6"/>
+    <tableColumn id="5" name="ADDRESS 2" dataDxfId="5"/>
+    <tableColumn id="6" name="ADDRESS 3" dataDxfId="4"/>
+    <tableColumn id="7" name="LATITUDE" dataDxfId="3"/>
+    <tableColumn id="8" name="LONGITUDE" dataDxfId="2"/>
+    <tableColumn id="9" name="POSTAL CODE" dataDxfId="1"/>
+    <tableColumn id="10" name="REVISION" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2671,8 +2695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="C270" workbookViewId="0">
+      <selection activeCell="J284" sqref="J284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2712,10 +2736,10 @@
       <c r="H1" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>526</v>
       </c>
     </row>
@@ -2744,8 +2768,11 @@
       <c r="H2" s="2">
         <v>109971901</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="1">
         <v>40355</v>
+      </c>
+      <c r="J2" s="1">
+        <v>78821</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2773,8 +2800,11 @@
       <c r="H3" s="1">
         <v>0</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="1">
         <v>17533</v>
+      </c>
+      <c r="J3" s="1">
+        <v>17530</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2802,8 +2832,11 @@
       <c r="H4" s="1">
         <v>0</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="1">
         <v>11430</v>
+      </c>
+      <c r="J4" s="1">
+        <v>11180</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2831,8 +2864,11 @@
       <c r="H5" s="1">
         <v>0</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="1">
         <v>16270</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2860,8 +2896,11 @@
       <c r="H6" s="1">
         <v>0</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="1">
         <v>17532</v>
+      </c>
+      <c r="J6" s="1">
+        <v>17530</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2889,8 +2928,11 @@
       <c r="H7" s="2">
         <v>10760553</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="1">
         <v>40791</v>
+      </c>
+      <c r="J7" s="1">
+        <v>40391</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2918,8 +2960,11 @@
       <c r="H8" s="1">
         <v>0</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="1">
         <v>41360</v>
+      </c>
+      <c r="J8" s="1">
+        <v>41361</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2947,8 +2992,11 @@
       <c r="H9" s="2">
         <v>107478382</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="1">
         <v>40714</v>
+      </c>
+      <c r="J9" s="1">
+        <v>40553</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2976,8 +3024,11 @@
       <c r="H10" s="1">
         <v>0</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="1">
         <v>39376</v>
+      </c>
+      <c r="J10" s="1">
+        <v>39372</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3005,8 +3056,11 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="1">
         <v>17532</v>
+      </c>
+      <c r="J11" s="1">
+        <v>17530</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -3034,8 +3088,11 @@
       <c r="H12" s="2">
         <v>107320233</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="1">
         <v>41322</v>
+      </c>
+      <c r="J12" s="1">
+        <v>41371</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -3063,8 +3120,11 @@
       <c r="H13" s="2">
         <v>107478382</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="1">
         <v>40716</v>
+      </c>
+      <c r="J13" s="1">
+        <v>40553</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -3092,8 +3152,11 @@
       <c r="H14" s="2">
         <v>106804564</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="1">
         <v>11430</v>
+      </c>
+      <c r="J14" s="1">
+        <v>11180</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -3121,8 +3184,11 @@
       <c r="H15" s="2">
         <v>107131467</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="1">
         <v>17550</v>
+      </c>
+      <c r="J15" s="1">
+        <v>17530</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -3150,11 +3216,14 @@
       <c r="H16" s="2">
         <v>106970494</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="1">
         <v>16826</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" s="1">
+        <v>16820</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>742</v>
       </c>
@@ -3179,11 +3248,14 @@
       <c r="H17" s="1">
         <v>0</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I17" s="1">
         <v>43260</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" s="1">
+        <v>43261</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>744</v>
       </c>
@@ -3208,11 +3280,14 @@
       <c r="H18" s="1">
         <v>0</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="1">
         <v>40352</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>795</v>
       </c>
@@ -3237,11 +3312,14 @@
       <c r="H19" s="2">
         <v>10611693</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="1">
         <v>42231</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19" s="1">
+        <v>42211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>841</v>
       </c>
@@ -3266,11 +3344,14 @@
       <c r="H20" s="2">
         <v>106872681</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I20" s="1">
         <v>16813</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" s="1">
+        <v>16810</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>861</v>
       </c>
@@ -3295,11 +3376,14 @@
       <c r="H21" s="2">
         <v>107075647</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I21" s="1">
         <v>17511</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" s="1">
+        <v>17510</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>863</v>
       </c>
@@ -3324,11 +3408,12 @@
       <c r="H22" s="2">
         <v>107293207</v>
       </c>
-      <c r="I22" s="5">
+      <c r="I22" s="1">
         <v>41334</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>873</v>
       </c>
@@ -3353,11 +3438,12 @@
       <c r="H23" s="1">
         <v>0</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I23" s="1">
         <v>11222</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>913</v>
       </c>
@@ -3382,11 +3468,12 @@
       <c r="H24" s="2">
         <v>106794241</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I24" s="1">
         <v>16472</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>917</v>
       </c>
@@ -3411,11 +3498,12 @@
       <c r="H25" s="2">
         <v>106592438</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="1">
         <v>15811</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>960</v>
       </c>
@@ -3440,11 +3528,14 @@
       <c r="H26" s="2">
         <v>107142544</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I26" s="1">
         <v>43260</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" s="1">
+        <v>43261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>980</v>
       </c>
@@ -3469,11 +3560,12 @@
       <c r="H27" s="2">
         <v>106592438</v>
       </c>
-      <c r="I27" s="5">
+      <c r="I27" s="1">
         <v>15811</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>996</v>
       </c>
@@ -3498,11 +3590,14 @@
       <c r="H28" s="2">
         <v>107131467</v>
       </c>
-      <c r="I28" s="5">
+      <c r="I28" s="1">
         <v>17550</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>999</v>
       </c>
@@ -3527,11 +3622,14 @@
       <c r="H29" s="1">
         <v>0</v>
       </c>
-      <c r="I29" s="5">
+      <c r="I29" s="1">
         <v>11430</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" s="1">
+        <v>11180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>1006</v>
       </c>
@@ -3556,11 +3654,12 @@
       <c r="H30" s="2">
         <v>106592438</v>
       </c>
-      <c r="I30" s="5">
+      <c r="I30" s="1">
         <v>15811</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>1034</v>
       </c>
@@ -3585,11 +3684,12 @@
       <c r="H31" s="2">
         <v>106868555</v>
       </c>
-      <c r="I31" s="5">
+      <c r="I31" s="1">
         <v>16952</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>1040</v>
       </c>
@@ -3614,11 +3714,14 @@
       <c r="H32" s="1">
         <v>0</v>
       </c>
-      <c r="I32" s="5">
+      <c r="I32" s="1">
         <v>17532</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="J32" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>1094</v>
       </c>
@@ -3643,11 +3746,14 @@
       <c r="H33" s="1">
         <v>0</v>
       </c>
-      <c r="I33" s="5">
+      <c r="I33" s="1">
         <v>39376</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33" s="1">
+        <v>39372</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>1099</v>
       </c>
@@ -3672,11 +3778,12 @@
       <c r="H34" s="2">
         <v>106055822</v>
       </c>
-      <c r="I34" s="5">
+      <c r="I34" s="1">
         <v>42435</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>1114</v>
       </c>
@@ -3701,11 +3808,14 @@
       <c r="H35" s="1">
         <v>0</v>
       </c>
-      <c r="I35" s="5">
+      <c r="I35" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>1146</v>
       </c>
@@ -3730,11 +3840,12 @@
       <c r="H36" s="2">
         <v>107619123</v>
       </c>
-      <c r="I36" s="5">
+      <c r="I36" s="1">
         <v>40298</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>1189</v>
       </c>
@@ -3759,11 +3870,12 @@
       <c r="H37" s="2">
         <v>107320233</v>
       </c>
-      <c r="I37" s="5">
+      <c r="I37" s="1">
         <v>41326</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>1200</v>
       </c>
@@ -3788,11 +3900,14 @@
       <c r="H38" s="2">
         <v>107187905</v>
       </c>
-      <c r="I38" s="5">
+      <c r="I38" s="1">
         <v>17533</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="J38" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>1225</v>
       </c>
@@ -3817,11 +3932,12 @@
       <c r="H39" s="1">
         <v>0</v>
       </c>
-      <c r="I39" s="5">
+      <c r="I39" s="1">
         <v>40199</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>1231</v>
       </c>
@@ -3846,11 +3962,12 @@
       <c r="H40" s="2">
         <v>107680431</v>
       </c>
-      <c r="I40" s="5">
+      <c r="I40" s="1">
         <v>40296</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>1237</v>
       </c>
@@ -3875,11 +3992,12 @@
       <c r="H41" s="1">
         <v>0</v>
       </c>
-      <c r="I41" s="5">
+      <c r="I41" s="1">
         <v>41180</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>1256</v>
       </c>
@@ -3904,11 +4022,12 @@
       <c r="H42" s="2">
         <v>107320233</v>
       </c>
-      <c r="I42" s="5">
+      <c r="I42" s="1">
         <v>41326</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>1289</v>
       </c>
@@ -3933,11 +4052,14 @@
       <c r="H43" s="1">
         <v>0</v>
       </c>
-      <c r="I43" s="5">
+      <c r="I43" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="J43" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>1304</v>
       </c>
@@ -3962,11 +4084,12 @@
       <c r="H44" s="1">
         <v>0</v>
       </c>
-      <c r="I44" s="5">
+      <c r="I44" s="1">
         <v>17534</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>1356</v>
       </c>
@@ -3991,11 +4114,12 @@
       <c r="H45" s="1">
         <v>0</v>
       </c>
-      <c r="I45" s="5">
+      <c r="I45" s="1">
         <v>15721</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>1358</v>
       </c>
@@ -4020,11 +4144,14 @@
       <c r="H46" s="2">
         <v>10760553</v>
       </c>
-      <c r="I46" s="5">
+      <c r="I46" s="1">
         <v>40791</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="J46" s="1">
+        <v>40391</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47">
         <v>1380</v>
       </c>
@@ -4049,11 +4176,12 @@
       <c r="H47" s="1">
         <v>0</v>
       </c>
-      <c r="I47" s="5">
+      <c r="I47" s="1">
         <v>17534</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>1389</v>
       </c>
@@ -4078,11 +4206,12 @@
       <c r="H48" s="1">
         <v>0</v>
       </c>
-      <c r="I48" s="5">
+      <c r="I48" s="1">
         <v>45159</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>1429</v>
       </c>
@@ -4107,11 +4236,12 @@
       <c r="H49" s="2">
         <v>106466619</v>
       </c>
-      <c r="I49" s="5">
+      <c r="I49" s="1">
         <v>16672</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>1433</v>
       </c>
@@ -4136,11 +4266,12 @@
       <c r="H50" s="1">
         <v>0</v>
       </c>
-      <c r="I50" s="5">
+      <c r="I50" s="1">
         <v>17534</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>1453</v>
       </c>
@@ -4165,11 +4296,12 @@
       <c r="H51" s="1">
         <v>0</v>
       </c>
-      <c r="I51" s="5">
+      <c r="I51" s="1">
         <v>15853</v>
       </c>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>1468</v>
       </c>
@@ -4194,11 +4326,14 @@
       <c r="H52" s="2">
         <v>107131467</v>
       </c>
-      <c r="I52" s="5">
+      <c r="I52" s="1">
         <v>17550</v>
       </c>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="J52" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>1469</v>
       </c>
@@ -4223,11 +4358,12 @@
       <c r="H53" s="2">
         <v>107169124</v>
       </c>
-      <c r="I53" s="5">
+      <c r="I53" s="1">
         <v>17534</v>
       </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>1501</v>
       </c>
@@ -4252,11 +4388,12 @@
       <c r="H54" s="1">
         <v>0</v>
       </c>
-      <c r="I54" s="5">
+      <c r="I54" s="1">
         <v>16270</v>
       </c>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55">
         <v>1505</v>
       </c>
@@ -4281,11 +4418,14 @@
       <c r="H55" s="2">
         <v>107131467</v>
       </c>
-      <c r="I55" s="5">
+      <c r="I55" s="1">
         <v>17550</v>
       </c>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="J55" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56">
         <v>1521</v>
       </c>
@@ -4310,11 +4450,12 @@
       <c r="H56" s="1">
         <v>0</v>
       </c>
-      <c r="I56" s="5">
+      <c r="I56" s="1">
         <v>16378</v>
       </c>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57">
         <v>1540</v>
       </c>
@@ -4339,11 +4480,12 @@
       <c r="H57" s="2">
         <v>107343161</v>
       </c>
-      <c r="I57" s="5">
+      <c r="I57" s="1">
         <v>40754</v>
       </c>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>1548</v>
       </c>
@@ -4368,11 +4510,12 @@
       <c r="H58" s="1">
         <v>0</v>
       </c>
-      <c r="I58" s="5">
+      <c r="I58" s="1">
         <v>15711</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59">
         <v>1603</v>
       </c>
@@ -4397,11 +4540,12 @@
       <c r="H59" s="2">
         <v>106868555</v>
       </c>
-      <c r="I59" s="5">
+      <c r="I59" s="1">
         <v>16952</v>
       </c>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60">
         <v>1610</v>
       </c>
@@ -4426,11 +4570,12 @@
       <c r="H60" s="2">
         <v>106595858</v>
       </c>
-      <c r="I60" s="5">
+      <c r="I60" s="1">
         <v>16285</v>
       </c>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61">
         <v>1625</v>
       </c>
@@ -4455,11 +4600,14 @@
       <c r="H61" s="2">
         <v>107131467</v>
       </c>
-      <c r="I61" s="5">
+      <c r="I61" s="1">
         <v>17550</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="J61" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62">
         <v>1674</v>
       </c>
@@ -4484,11 +4632,14 @@
       <c r="H62" s="1">
         <v>0</v>
       </c>
-      <c r="I62" s="5">
+      <c r="I62" s="1">
         <v>43260</v>
       </c>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="J62" s="1">
+        <v>43261</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63">
         <v>1699</v>
       </c>
@@ -4513,11 +4664,12 @@
       <c r="H63" s="2">
         <v>106872681</v>
       </c>
-      <c r="I63" s="5">
+      <c r="I63" s="1">
         <v>16811</v>
       </c>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64">
         <v>1712</v>
       </c>
@@ -4542,11 +4694,12 @@
       <c r="H64" s="1">
         <v>0</v>
       </c>
-      <c r="I64" s="5">
+      <c r="I64" s="1">
         <v>43286</v>
       </c>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="J64" s="1"/>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65">
         <v>1714</v>
       </c>
@@ -4571,11 +4724,12 @@
       <c r="H65" s="2">
         <v>109971901</v>
       </c>
-      <c r="I65" s="5">
+      <c r="I65" s="1">
         <v>40355</v>
       </c>
-    </row>
-    <row r="66" spans="1:9">
+      <c r="J65" s="1"/>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66">
         <v>1732</v>
       </c>
@@ -4600,11 +4754,12 @@
       <c r="H66" s="2">
         <v>106677936</v>
       </c>
-      <c r="I66" s="5">
+      <c r="I66" s="1">
         <v>16387</v>
       </c>
-    </row>
-    <row r="67" spans="1:9">
+      <c r="J66" s="1"/>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67">
         <v>1753</v>
       </c>
@@ -4629,11 +4784,14 @@
       <c r="H67" s="2">
         <v>107131467</v>
       </c>
-      <c r="I67" s="5">
+      <c r="I67" s="1">
         <v>17550</v>
       </c>
-    </row>
-    <row r="68" spans="1:9">
+      <c r="J67" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68">
         <v>1814</v>
       </c>
@@ -4658,11 +4816,12 @@
       <c r="H68" s="2">
         <v>106956857</v>
       </c>
-      <c r="I68" s="5">
+      <c r="I68" s="1">
         <v>16872</v>
       </c>
-    </row>
-    <row r="69" spans="1:9">
+      <c r="J68" s="1"/>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69">
         <v>1815</v>
       </c>
@@ -4687,11 +4846,12 @@
       <c r="H69" s="2">
         <v>106892647</v>
       </c>
-      <c r="I69" s="5">
+      <c r="I69" s="1">
         <v>16772</v>
       </c>
-    </row>
-    <row r="70" spans="1:9">
+      <c r="J69" s="1"/>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70">
         <v>1816</v>
       </c>
@@ -4716,11 +4876,14 @@
       <c r="H70" s="1">
         <v>0</v>
       </c>
-      <c r="I70" s="5">
+      <c r="I70" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="71" spans="1:9">
+      <c r="J70" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71">
         <v>1846</v>
       </c>
@@ -4745,11 +4908,12 @@
       <c r="H71" s="2">
         <v>107436089</v>
       </c>
-      <c r="I71" s="5">
+      <c r="I71" s="1">
         <v>40762</v>
       </c>
-    </row>
-    <row r="72" spans="1:9">
+      <c r="J71" s="1"/>
+    </row>
+    <row r="72" spans="1:10">
       <c r="A72">
         <v>1867</v>
       </c>
@@ -4774,11 +4938,12 @@
       <c r="H72" s="2">
         <v>107293207</v>
       </c>
-      <c r="I72" s="5">
+      <c r="I72" s="1">
         <v>16831</v>
       </c>
-    </row>
-    <row r="73" spans="1:9">
+      <c r="J72" s="1"/>
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73">
         <v>1875</v>
       </c>
@@ -4803,11 +4968,14 @@
       <c r="H73" s="1">
         <v>0</v>
       </c>
-      <c r="I73" s="5">
+      <c r="I73" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="74" spans="1:9">
+      <c r="J73" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74">
         <v>1883</v>
       </c>
@@ -4832,11 +5000,12 @@
       <c r="H74" s="2">
         <v>107634157</v>
       </c>
-      <c r="I74" s="5">
+      <c r="I74" s="1">
         <v>40354</v>
       </c>
-    </row>
-    <row r="75" spans="1:9">
+      <c r="J74" s="1"/>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75">
         <v>1886</v>
       </c>
@@ -4861,11 +5030,12 @@
       <c r="H75" s="2">
         <v>10679706</v>
       </c>
-      <c r="I75" s="5">
+      <c r="I75" s="1">
         <v>16785</v>
       </c>
-    </row>
-    <row r="76" spans="1:9">
+      <c r="J75" s="1"/>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76">
         <v>1919</v>
       </c>
@@ -4890,11 +5060,14 @@
       <c r="H76" s="2">
         <v>107075647</v>
       </c>
-      <c r="I76" s="5">
+      <c r="I76" s="1">
         <v>17511</v>
       </c>
-    </row>
-    <row r="77" spans="1:9">
+      <c r="J76" s="1">
+        <v>17510</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77">
         <v>1954</v>
       </c>
@@ -4919,11 +5092,12 @@
       <c r="H77" s="1">
         <v>0</v>
       </c>
-      <c r="I77" s="5">
+      <c r="I77" s="1">
         <v>15721</v>
       </c>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="J77" s="1"/>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78">
         <v>1987</v>
       </c>
@@ -4948,11 +5122,12 @@
       <c r="H78" s="2">
         <v>106932287</v>
       </c>
-      <c r="I78" s="5">
+      <c r="I78" s="1">
         <v>16759</v>
       </c>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="J78" s="1"/>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79">
         <v>1992</v>
       </c>
@@ -4977,11 +5152,12 @@
       <c r="H79" s="2">
         <v>108433197</v>
       </c>
-      <c r="I79" s="5">
+      <c r="I79" s="1">
         <v>45160</v>
       </c>
-    </row>
-    <row r="80" spans="1:9">
+      <c r="J79" s="1"/>
+    </row>
+    <row r="80" spans="1:10">
       <c r="A80">
         <v>2061</v>
       </c>
@@ -5006,11 +5182,14 @@
       <c r="H80" s="2">
         <v>107321461</v>
       </c>
-      <c r="I80" s="5">
+      <c r="I80" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="J80" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81">
         <v>2066</v>
       </c>
@@ -5035,11 +5214,12 @@
       <c r="H81" s="2">
         <v>10680014</v>
       </c>
-      <c r="I81" s="5">
+      <c r="I81" s="1">
         <v>16927</v>
       </c>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="J81" s="1"/>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82">
         <v>2072</v>
       </c>
@@ -5064,11 +5244,12 @@
       <c r="H82" s="2">
         <v>107673327</v>
       </c>
-      <c r="I82" s="5">
+      <c r="I82" s="1">
         <v>40193</v>
       </c>
-    </row>
-    <row r="83" spans="1:9">
+      <c r="J82" s="1"/>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83">
         <v>2197</v>
       </c>
@@ -5093,11 +5274,12 @@
       <c r="H83" s="1">
         <v>0</v>
       </c>
-      <c r="I83" s="5">
+      <c r="I83" s="1">
         <v>17163</v>
       </c>
-    </row>
-    <row r="84" spans="1:9">
+      <c r="J83" s="1"/>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84">
         <v>2207</v>
       </c>
@@ -5122,11 +5304,12 @@
       <c r="H84" s="2">
         <v>106845739</v>
       </c>
-      <c r="I84" s="5">
+      <c r="I84" s="1">
         <v>16951</v>
       </c>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="J84" s="1"/>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85">
         <v>2364</v>
       </c>
@@ -5151,11 +5334,14 @@
       <c r="H85" s="2">
         <v>107478382</v>
       </c>
-      <c r="I85" s="5">
+      <c r="I85" s="1">
         <v>40714</v>
       </c>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="J85" s="1">
+        <v>40553</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86">
         <v>2472</v>
       </c>
@@ -5180,11 +5366,12 @@
       <c r="H86" s="2">
         <v>107418781</v>
       </c>
-      <c r="I86" s="5">
+      <c r="I86" s="1">
         <v>40974</v>
       </c>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="J86" s="1"/>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87">
         <v>2476</v>
       </c>
@@ -5209,11 +5396,14 @@
       <c r="H87" s="2">
         <v>107321458</v>
       </c>
-      <c r="I87" s="5">
+      <c r="I87" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="J87" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88">
         <v>2488</v>
       </c>
@@ -5238,11 +5428,12 @@
       <c r="H88" s="2">
         <v>106872681</v>
       </c>
-      <c r="I88" s="5">
+      <c r="I88" s="1">
         <v>16811</v>
       </c>
-    </row>
-    <row r="89" spans="1:9">
+      <c r="J88" s="1"/>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89">
         <v>2516</v>
       </c>
@@ -5267,11 +5458,12 @@
       <c r="H89" s="2">
         <v>106872681</v>
       </c>
-      <c r="I89" s="5">
+      <c r="I89" s="1">
         <v>16811</v>
       </c>
-    </row>
-    <row r="90" spans="1:9">
+      <c r="J89" s="1"/>
+    </row>
+    <row r="90" spans="1:10">
       <c r="A90">
         <v>2517</v>
       </c>
@@ -5296,11 +5488,12 @@
       <c r="H90" s="2">
         <v>106872681</v>
       </c>
-      <c r="I90" s="5">
+      <c r="I90" s="1">
         <v>16811</v>
       </c>
-    </row>
-    <row r="91" spans="1:9">
+      <c r="J90" s="1"/>
+    </row>
+    <row r="91" spans="1:10">
       <c r="A91">
         <v>2529</v>
       </c>
@@ -5325,11 +5518,12 @@
       <c r="H91" s="1">
         <v>0</v>
       </c>
-      <c r="I91" s="5">
+      <c r="I91" s="1">
         <v>15711</v>
       </c>
-    </row>
-    <row r="92" spans="1:9">
+      <c r="J91" s="1"/>
+    </row>
+    <row r="92" spans="1:10">
       <c r="A92">
         <v>2545</v>
       </c>
@@ -5354,11 +5548,12 @@
       <c r="H92" s="1">
         <v>0</v>
       </c>
-      <c r="I92" s="5">
+      <c r="I92" s="1">
         <v>16661</v>
       </c>
-    </row>
-    <row r="93" spans="1:9">
+      <c r="J92" s="1"/>
+    </row>
+    <row r="93" spans="1:10">
       <c r="A93">
         <v>2576</v>
       </c>
@@ -5383,11 +5578,12 @@
       <c r="H93" s="1">
         <v>0</v>
       </c>
-      <c r="I93" s="5">
+      <c r="I93" s="1">
         <v>40560</v>
       </c>
-    </row>
-    <row r="94" spans="1:9">
+      <c r="J93" s="1"/>
+    </row>
+    <row r="94" spans="1:10">
       <c r="A94">
         <v>2577</v>
       </c>
@@ -5412,11 +5608,12 @@
       <c r="H94" s="1">
         <v>0</v>
       </c>
-      <c r="I94" s="5">
+      <c r="I94" s="1">
         <v>44179</v>
       </c>
-    </row>
-    <row r="95" spans="1:9">
+      <c r="J94" s="1"/>
+    </row>
+    <row r="95" spans="1:10">
       <c r="A95">
         <v>2598</v>
       </c>
@@ -5441,11 +5638,12 @@
       <c r="H95" s="2">
         <v>106579602</v>
       </c>
-      <c r="I95" s="5">
+      <c r="I95" s="1">
         <v>15561</v>
       </c>
-    </row>
-    <row r="96" spans="1:9">
+      <c r="J95" s="1"/>
+    </row>
+    <row r="96" spans="1:10">
       <c r="A96">
         <v>2603</v>
       </c>
@@ -5470,11 +5668,12 @@
       <c r="H96" s="1">
         <v>0</v>
       </c>
-      <c r="I96" s="5">
+      <c r="I96" s="1">
         <v>17631</v>
       </c>
-    </row>
-    <row r="97" spans="1:9">
+      <c r="J96" s="1"/>
+    </row>
+    <row r="97" spans="1:10">
       <c r="A97">
         <v>2636</v>
       </c>
@@ -5499,11 +5698,12 @@
       <c r="H97" s="1">
         <v>0</v>
       </c>
-      <c r="I97" s="5">
+      <c r="I97" s="1">
         <v>46191</v>
       </c>
-    </row>
-    <row r="98" spans="1:9">
+      <c r="J97" s="1"/>
+    </row>
+    <row r="98" spans="1:10">
       <c r="A98">
         <v>2638</v>
       </c>
@@ -5528,11 +5728,14 @@
       <c r="H98" s="2">
         <v>107121992</v>
       </c>
-      <c r="I98" s="5">
+      <c r="I98" s="1">
         <v>17532</v>
       </c>
-    </row>
-    <row r="99" spans="1:9">
+      <c r="J98" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
       <c r="A99">
         <v>2658</v>
       </c>
@@ -5557,11 +5760,12 @@
       <c r="H99" s="2">
         <v>107680431</v>
       </c>
-      <c r="I99" s="5">
+      <c r="I99" s="1">
         <v>40296</v>
       </c>
-    </row>
-    <row r="100" spans="1:9">
+      <c r="J99" s="1"/>
+    </row>
+    <row r="100" spans="1:10">
       <c r="A100">
         <v>2674</v>
       </c>
@@ -5586,11 +5790,14 @@
       <c r="H100" s="2">
         <v>107121992</v>
       </c>
-      <c r="I100" s="5">
+      <c r="I100" s="1">
         <v>17532</v>
       </c>
-    </row>
-    <row r="101" spans="1:9">
+      <c r="J100" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
       <c r="A101">
         <v>2676</v>
       </c>
@@ -5615,11 +5822,12 @@
       <c r="H101" s="1">
         <v>0</v>
       </c>
-      <c r="I101" s="5">
+      <c r="I101" s="1">
         <v>41375</v>
       </c>
-    </row>
-    <row r="102" spans="1:9">
+      <c r="J101" s="1"/>
+    </row>
+    <row r="102" spans="1:10">
       <c r="A102">
         <v>2679</v>
       </c>
@@ -5644,11 +5852,12 @@
       <c r="H102" s="1">
         <v>0</v>
       </c>
-      <c r="I102" s="5">
+      <c r="I102" s="1">
         <v>45159</v>
       </c>
-    </row>
-    <row r="103" spans="1:9">
+      <c r="J102" s="1"/>
+    </row>
+    <row r="103" spans="1:10">
       <c r="A103">
         <v>2694</v>
       </c>
@@ -5673,11 +5882,12 @@
       <c r="H103" s="1">
         <v>0</v>
       </c>
-      <c r="I103" s="5">
+      <c r="I103" s="1">
         <v>15611</v>
       </c>
-    </row>
-    <row r="104" spans="1:9">
+      <c r="J103" s="1"/>
+    </row>
+    <row r="104" spans="1:10">
       <c r="A104">
         <v>2727</v>
       </c>
@@ -5702,11 +5912,14 @@
       <c r="H104" s="2">
         <v>107121992</v>
       </c>
-      <c r="I104" s="5">
+      <c r="I104" s="1">
         <v>17532</v>
       </c>
-    </row>
-    <row r="105" spans="1:9">
+      <c r="J104" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
       <c r="A105">
         <v>2847</v>
       </c>
@@ -5731,11 +5944,12 @@
       <c r="H105" s="1">
         <v>0</v>
       </c>
-      <c r="I105" s="5">
+      <c r="I105" s="1">
         <v>41180</v>
       </c>
-    </row>
-    <row r="106" spans="1:9">
+      <c r="J105" s="1"/>
+    </row>
+    <row r="106" spans="1:10">
       <c r="A106">
         <v>2871</v>
       </c>
@@ -5760,11 +5974,14 @@
       <c r="H106" s="2">
         <v>107075647</v>
       </c>
-      <c r="I106" s="5">
+      <c r="I106" s="1">
         <v>17511</v>
       </c>
-    </row>
-    <row r="107" spans="1:9">
+      <c r="J106" s="1">
+        <v>17510</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10">
       <c r="A107">
         <v>2896</v>
       </c>
@@ -5789,11 +6006,12 @@
       <c r="H107" s="1">
         <v>0</v>
       </c>
-      <c r="I107" s="5">
+      <c r="I107" s="1">
         <v>45360</v>
       </c>
-    </row>
-    <row r="108" spans="1:9">
+      <c r="J107" s="1"/>
+    </row>
+    <row r="108" spans="1:10">
       <c r="A108">
         <v>2897</v>
       </c>
@@ -5818,11 +6036,12 @@
       <c r="H108" s="2">
         <v>107436089</v>
       </c>
-      <c r="I108" s="5">
+      <c r="I108" s="1">
         <v>40567</v>
       </c>
-    </row>
-    <row r="109" spans="1:9">
+      <c r="J108" s="1"/>
+    </row>
+    <row r="109" spans="1:10">
       <c r="A109">
         <v>2902</v>
       </c>
@@ -5847,11 +6066,12 @@
       <c r="H109" s="1">
         <v>0</v>
       </c>
-      <c r="I109" s="5">
+      <c r="I109" s="1">
         <v>44150</v>
       </c>
-    </row>
-    <row r="110" spans="1:9">
+      <c r="J109" s="1"/>
+    </row>
+    <row r="110" spans="1:10">
       <c r="A110">
         <v>2912</v>
       </c>
@@ -5876,11 +6096,14 @@
       <c r="H110" s="1">
         <v>0</v>
       </c>
-      <c r="I110" s="5">
+      <c r="I110" s="1">
         <v>17532</v>
       </c>
-    </row>
-    <row r="111" spans="1:9">
+      <c r="J110" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
       <c r="A111">
         <v>2913</v>
       </c>
@@ -5905,11 +6128,12 @@
       <c r="H111" s="2">
         <v>11268212</v>
       </c>
-      <c r="I111" s="5">
+      <c r="I111" s="1">
         <v>60168</v>
       </c>
-    </row>
-    <row r="112" spans="1:9">
+      <c r="J111" s="1"/>
+    </row>
+    <row r="112" spans="1:10">
       <c r="A112">
         <v>2928</v>
       </c>
@@ -5934,11 +6158,12 @@
       <c r="H112" s="2">
         <v>107471637</v>
       </c>
-      <c r="I112" s="5">
+      <c r="I112" s="1">
         <v>41376</v>
       </c>
-    </row>
-    <row r="113" spans="1:9">
+      <c r="J112" s="1"/>
+    </row>
+    <row r="113" spans="1:10">
       <c r="A113">
         <v>2934</v>
       </c>
@@ -5963,11 +6188,14 @@
       <c r="H113" s="2">
         <v>107075647</v>
       </c>
-      <c r="I113" s="5">
+      <c r="I113" s="1">
         <v>17511</v>
       </c>
-    </row>
-    <row r="114" spans="1:9">
+      <c r="J113" s="1">
+        <v>17510</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
       <c r="A114">
         <v>2937</v>
       </c>
@@ -5992,11 +6220,14 @@
       <c r="H114" s="2">
         <v>107321458</v>
       </c>
-      <c r="I114" s="5">
+      <c r="I114" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="115" spans="1:9">
+      <c r="J114" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10">
       <c r="A115">
         <v>2954</v>
       </c>
@@ -6021,11 +6252,12 @@
       <c r="H115" s="2">
         <v>107214401</v>
       </c>
-      <c r="I115" s="5">
+      <c r="I115" s="1">
         <v>41364</v>
       </c>
-    </row>
-    <row r="116" spans="1:9">
+      <c r="J115" s="1"/>
+    </row>
+    <row r="116" spans="1:10">
       <c r="A116">
         <v>3029</v>
       </c>
@@ -6050,11 +6282,12 @@
       <c r="H116" s="2">
         <v>107158466</v>
       </c>
-      <c r="I116" s="5">
+      <c r="I116" s="1">
         <v>17535</v>
       </c>
-    </row>
-    <row r="117" spans="1:9">
+      <c r="J116" s="1"/>
+    </row>
+    <row r="117" spans="1:10">
       <c r="A117">
         <v>3041</v>
       </c>
@@ -6079,11 +6312,12 @@
       <c r="H117" s="1">
         <v>0</v>
       </c>
-      <c r="I117" s="5">
+      <c r="I117" s="1">
         <v>15532</v>
       </c>
-    </row>
-    <row r="118" spans="1:9">
+      <c r="J117" s="1"/>
+    </row>
+    <row r="118" spans="1:10">
       <c r="A118">
         <v>3053</v>
       </c>
@@ -6108,11 +6342,14 @@
       <c r="H118" s="1">
         <v>0</v>
       </c>
-      <c r="I118" s="5">
+      <c r="I118" s="1">
         <v>17533</v>
       </c>
-    </row>
-    <row r="119" spans="1:9">
+      <c r="J118" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
       <c r="A119">
         <v>3069</v>
       </c>
@@ -6137,11 +6374,14 @@
       <c r="H119" s="2">
         <v>107321458</v>
       </c>
-      <c r="I119" s="5">
+      <c r="I119" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="120" spans="1:9">
+      <c r="J119" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10">
       <c r="A120">
         <v>3112</v>
       </c>
@@ -6166,11 +6406,14 @@
       <c r="H120" s="2">
         <v>107321458</v>
       </c>
-      <c r="I120" s="5">
+      <c r="I120" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="121" spans="1:9">
+      <c r="J120" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
       <c r="A121">
         <v>3129</v>
       </c>
@@ -6195,11 +6438,12 @@
       <c r="H121" s="1">
         <v>0</v>
       </c>
-      <c r="I121" s="5">
+      <c r="I121" s="1">
         <v>17631</v>
       </c>
-    </row>
-    <row r="122" spans="1:9">
+      <c r="J121" s="1"/>
+    </row>
+    <row r="122" spans="1:10">
       <c r="A122">
         <v>3139</v>
       </c>
@@ -6224,11 +6468,14 @@
       <c r="H122" s="2">
         <v>107187905</v>
       </c>
-      <c r="I122" s="5">
+      <c r="I122" s="1">
         <v>17533</v>
       </c>
-    </row>
-    <row r="123" spans="1:9">
+      <c r="J122" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
       <c r="A123">
         <v>3140</v>
       </c>
@@ -6253,11 +6500,12 @@
       <c r="H123" s="1">
         <v>0</v>
       </c>
-      <c r="I123" s="5">
+      <c r="I123" s="1">
         <v>17621</v>
       </c>
-    </row>
-    <row r="124" spans="1:9">
+      <c r="J123" s="1"/>
+    </row>
+    <row r="124" spans="1:10">
       <c r="A124">
         <v>3154</v>
       </c>
@@ -6282,11 +6530,14 @@
       <c r="H124" s="1">
         <v>0</v>
       </c>
-      <c r="I124" s="5">
+      <c r="I124" s="1">
         <v>17532</v>
       </c>
-    </row>
-    <row r="125" spans="1:9">
+      <c r="J124" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
       <c r="A125">
         <v>3178</v>
       </c>
@@ -6311,11 +6562,14 @@
       <c r="H125" s="1">
         <v>0</v>
       </c>
-      <c r="I125" s="5">
+      <c r="I125" s="1">
         <v>17533</v>
       </c>
-    </row>
-    <row r="126" spans="1:9">
+      <c r="J125" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10">
       <c r="A126">
         <v>3195</v>
       </c>
@@ -6340,11 +6594,12 @@
       <c r="H126" s="2">
         <v>106592438</v>
       </c>
-      <c r="I126" s="5">
+      <c r="I126" s="1">
         <v>15811</v>
       </c>
-    </row>
-    <row r="127" spans="1:9">
+      <c r="J126" s="1"/>
+    </row>
+    <row r="127" spans="1:10">
       <c r="A127">
         <v>3209</v>
       </c>
@@ -6369,11 +6624,12 @@
       <c r="H127" s="2">
         <v>107680431</v>
       </c>
-      <c r="I127" s="5">
+      <c r="I127" s="1">
         <v>40296</v>
       </c>
-    </row>
-    <row r="128" spans="1:9">
+      <c r="J127" s="1"/>
+    </row>
+    <row r="128" spans="1:10">
       <c r="A128">
         <v>3217</v>
       </c>
@@ -6398,11 +6654,12 @@
       <c r="H128" s="1">
         <v>0</v>
       </c>
-      <c r="I128" s="5">
+      <c r="I128" s="1">
         <v>44150</v>
       </c>
-    </row>
-    <row r="129" spans="1:9">
+      <c r="J128" s="1"/>
+    </row>
+    <row r="129" spans="1:10">
       <c r="A129">
         <v>3231</v>
       </c>
@@ -6427,11 +6684,12 @@
       <c r="H129" s="1">
         <v>0</v>
       </c>
-      <c r="I129" s="5">
+      <c r="I129" s="1">
         <v>15721</v>
       </c>
-    </row>
-    <row r="130" spans="1:9">
+      <c r="J129" s="1"/>
+    </row>
+    <row r="130" spans="1:10">
       <c r="A130">
         <v>3319</v>
       </c>
@@ -6456,11 +6714,12 @@
       <c r="H130" s="1">
         <v>0</v>
       </c>
-      <c r="I130" s="5">
+      <c r="I130" s="1">
         <v>51157</v>
       </c>
-    </row>
-    <row r="131" spans="1:9">
+      <c r="J130" s="1"/>
+    </row>
+    <row r="131" spans="1:10">
       <c r="A131">
         <v>3380</v>
       </c>
@@ -6485,11 +6744,12 @@
       <c r="H131" s="2">
         <v>106837012</v>
       </c>
-      <c r="I131" s="5">
+      <c r="I131" s="1">
         <v>12610</v>
       </c>
-    </row>
-    <row r="132" spans="1:9">
+      <c r="J131" s="1"/>
+    </row>
+    <row r="132" spans="1:10">
       <c r="A132">
         <v>3419</v>
       </c>
@@ -6514,11 +6774,12 @@
       <c r="H132" s="1">
         <v>0</v>
       </c>
-      <c r="I132" s="5">
+      <c r="I132" s="1">
         <v>61728</v>
       </c>
-    </row>
-    <row r="133" spans="1:9">
+      <c r="J132" s="1"/>
+    </row>
+    <row r="133" spans="1:10">
       <c r="A133">
         <v>3446</v>
       </c>
@@ -6543,11 +6804,12 @@
       <c r="H133" s="1">
         <v>0</v>
       </c>
-      <c r="I133" s="5">
+      <c r="I133" s="1">
         <v>57771</v>
       </c>
-    </row>
-    <row r="134" spans="1:9">
+      <c r="J133" s="1"/>
+    </row>
+    <row r="134" spans="1:10">
       <c r="A134">
         <v>3454</v>
       </c>
@@ -6572,11 +6834,12 @@
       <c r="H134" s="2">
         <v>112106021</v>
       </c>
-      <c r="I134" s="5">
+      <c r="I134" s="1">
         <v>67724</v>
       </c>
-    </row>
-    <row r="135" spans="1:9">
+      <c r="J134" s="1"/>
+    </row>
+    <row r="135" spans="1:10">
       <c r="A135">
         <v>3526</v>
       </c>
@@ -6601,11 +6864,12 @@
       <c r="H135" s="2">
         <v>112462089</v>
       </c>
-      <c r="I135" s="5">
+      <c r="I135" s="1">
         <v>61301</v>
       </c>
-    </row>
-    <row r="136" spans="1:9">
+      <c r="J135" s="1"/>
+    </row>
+    <row r="136" spans="1:10">
       <c r="A136">
         <v>3577</v>
       </c>
@@ -6630,11 +6894,12 @@
       <c r="H136" s="2">
         <v>112462089</v>
       </c>
-      <c r="I136" s="5">
+      <c r="I136" s="1">
         <v>61301</v>
       </c>
-    </row>
-    <row r="137" spans="1:9">
+      <c r="J136" s="1"/>
+    </row>
+    <row r="137" spans="1:10">
       <c r="A137">
         <v>3638</v>
       </c>
@@ -6659,11 +6924,12 @@
       <c r="H137" s="2">
         <v>111901515</v>
       </c>
-      <c r="I137" s="5">
+      <c r="I137" s="1">
         <v>64412</v>
       </c>
-    </row>
-    <row r="138" spans="1:9">
+      <c r="J137" s="1"/>
+    </row>
+    <row r="138" spans="1:10">
       <c r="A138">
         <v>3820</v>
       </c>
@@ -6688,11 +6954,12 @@
       <c r="H138" s="2">
         <v>110986694</v>
       </c>
-      <c r="I138" s="5">
+      <c r="I138" s="1">
         <v>57771</v>
       </c>
-    </row>
-    <row r="139" spans="1:9">
+      <c r="J138" s="1"/>
+    </row>
+    <row r="139" spans="1:10">
       <c r="A139">
         <v>3838</v>
       </c>
@@ -6717,11 +6984,12 @@
       <c r="H139" s="1">
         <v>0</v>
       </c>
-      <c r="I139" s="5">
+      <c r="I139" s="1">
         <v>45126</v>
       </c>
-    </row>
-    <row r="140" spans="1:9">
+      <c r="J139" s="1"/>
+    </row>
+    <row r="140" spans="1:10">
       <c r="A140">
         <v>3912</v>
       </c>
@@ -6746,11 +7014,12 @@
       <c r="H140" s="1">
         <v>0</v>
       </c>
-      <c r="I140" s="5">
+      <c r="I140" s="1">
         <v>61532</v>
       </c>
-    </row>
-    <row r="141" spans="1:9">
+      <c r="J140" s="1"/>
+    </row>
+    <row r="141" spans="1:10">
       <c r="A141">
         <v>3942</v>
       </c>
@@ -6775,11 +7044,12 @@
       <c r="H141" s="1">
         <v>0</v>
       </c>
-      <c r="I141" s="5">
+      <c r="I141" s="1">
         <v>57771</v>
       </c>
-    </row>
-    <row r="142" spans="1:9">
+      <c r="J141" s="1"/>
+    </row>
+    <row r="142" spans="1:10">
       <c r="A142">
         <v>3944</v>
       </c>
@@ -6804,11 +7074,12 @@
       <c r="H142" s="1">
         <v>0</v>
       </c>
-      <c r="I142" s="5">
+      <c r="I142" s="1">
         <v>57771</v>
       </c>
-    </row>
-    <row r="143" spans="1:9">
+      <c r="J142" s="1"/>
+    </row>
+    <row r="143" spans="1:10">
       <c r="A143">
         <v>4075</v>
       </c>
@@ -6833,11 +7104,14 @@
       <c r="H143" s="2">
         <v>107321458</v>
       </c>
-      <c r="I143" s="5">
+      <c r="I143" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="144" spans="1:9">
+      <c r="J143" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10">
       <c r="A144">
         <v>4190</v>
       </c>
@@ -6862,11 +7136,12 @@
       <c r="H144" s="2">
         <v>111901515</v>
       </c>
-      <c r="I144" s="5">
+      <c r="I144" s="1">
         <v>64412</v>
       </c>
-    </row>
-    <row r="145" spans="1:9">
+      <c r="J144" s="1"/>
+    </row>
+    <row r="145" spans="1:10">
       <c r="A145">
         <v>4253</v>
       </c>
@@ -6891,11 +7166,12 @@
       <c r="H145" s="2">
         <v>111901515</v>
       </c>
-      <c r="I145" s="5">
+      <c r="I145" s="1">
         <v>64412</v>
       </c>
-    </row>
-    <row r="146" spans="1:9">
+      <c r="J145" s="1"/>
+    </row>
+    <row r="146" spans="1:10">
       <c r="A146">
         <v>4339</v>
       </c>
@@ -6920,11 +7196,12 @@
       <c r="H146" s="1">
         <v>0</v>
       </c>
-      <c r="I146" s="5">
+      <c r="I146" s="1">
         <v>41288</v>
       </c>
-    </row>
-    <row r="147" spans="1:9">
+      <c r="J146" s="1"/>
+    </row>
+    <row r="147" spans="1:10">
       <c r="A147">
         <v>4352</v>
       </c>
@@ -6949,11 +7226,12 @@
       <c r="H147" s="2">
         <v>106872681</v>
       </c>
-      <c r="I147" s="5">
+      <c r="I147" s="1">
         <v>16811</v>
       </c>
-    </row>
-    <row r="148" spans="1:9">
+      <c r="J147" s="1"/>
+    </row>
+    <row r="148" spans="1:10">
       <c r="A148">
         <v>4353</v>
       </c>
@@ -6978,11 +7256,12 @@
       <c r="H148" s="2">
         <v>112424676</v>
       </c>
-      <c r="I148" s="5">
+      <c r="I148" s="1">
         <v>61326</v>
       </c>
-    </row>
-    <row r="149" spans="1:9">
+      <c r="J148" s="1"/>
+    </row>
+    <row r="149" spans="1:10">
       <c r="A149">
         <v>4379</v>
       </c>
@@ -7007,11 +7286,12 @@
       <c r="H149" s="1">
         <v>0</v>
       </c>
-      <c r="I149" s="5">
+      <c r="I149" s="1">
         <v>57771</v>
       </c>
-    </row>
-    <row r="150" spans="1:9">
+      <c r="J149" s="1"/>
+    </row>
+    <row r="150" spans="1:10">
       <c r="A150">
         <v>4388</v>
       </c>
@@ -7036,11 +7316,12 @@
       <c r="H150" s="1">
         <v>0</v>
       </c>
-      <c r="I150" s="5">
+      <c r="I150" s="1">
         <v>55501</v>
       </c>
-    </row>
-    <row r="151" spans="1:9">
+      <c r="J150" s="1"/>
+    </row>
+    <row r="151" spans="1:10">
       <c r="A151">
         <v>4411</v>
       </c>
@@ -7065,11 +7346,12 @@
       <c r="H151" s="2">
         <v>106872681</v>
       </c>
-      <c r="I151" s="5">
+      <c r="I151" s="1">
         <v>16811</v>
       </c>
-    </row>
-    <row r="152" spans="1:9">
+      <c r="J151" s="1"/>
+    </row>
+    <row r="152" spans="1:10">
       <c r="A152">
         <v>4462</v>
       </c>
@@ -7094,11 +7376,12 @@
       <c r="H152" s="1">
         <v>0</v>
       </c>
-      <c r="I152" s="5">
+      <c r="I152" s="1">
         <v>61251</v>
       </c>
-    </row>
-    <row r="153" spans="1:9">
+      <c r="J152" s="1"/>
+    </row>
+    <row r="153" spans="1:10">
       <c r="A153">
         <v>4470</v>
       </c>
@@ -7123,11 +7406,12 @@
       <c r="H153" s="2">
         <v>107735029</v>
       </c>
-      <c r="I153" s="5">
+      <c r="I153" s="1">
         <v>41287</v>
       </c>
-    </row>
-    <row r="154" spans="1:9">
+      <c r="J153" s="1"/>
+    </row>
+    <row r="154" spans="1:10">
       <c r="A154">
         <v>4530</v>
       </c>
@@ -7152,11 +7436,14 @@
       <c r="H154" s="1">
         <v>0</v>
       </c>
-      <c r="I154" s="5">
+      <c r="I154" s="1">
         <v>17532</v>
       </c>
-    </row>
-    <row r="155" spans="1:9">
+      <c r="J154" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10">
       <c r="A155">
         <v>4548</v>
       </c>
@@ -7181,11 +7468,14 @@
       <c r="H155" s="2">
         <v>107321458</v>
       </c>
-      <c r="I155" s="5">
+      <c r="I155" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="156" spans="1:9">
+      <c r="J155" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10">
       <c r="A156">
         <v>4552</v>
       </c>
@@ -7210,11 +7500,12 @@
       <c r="H156" s="1">
         <v>0</v>
       </c>
-      <c r="I156" s="5">
+      <c r="I156" s="1">
         <v>57771</v>
       </c>
-    </row>
-    <row r="157" spans="1:9">
+      <c r="J156" s="1"/>
+    </row>
+    <row r="157" spans="1:10">
       <c r="A157">
         <v>4570</v>
       </c>
@@ -7239,11 +7530,12 @@
       <c r="H157" s="1">
         <v>0</v>
       </c>
-      <c r="I157" s="5">
+      <c r="I157" s="1">
         <v>57771</v>
       </c>
-    </row>
-    <row r="158" spans="1:9">
+      <c r="J157" s="1"/>
+    </row>
+    <row r="158" spans="1:10">
       <c r="A158">
         <v>4670</v>
       </c>
@@ -7268,11 +7560,14 @@
       <c r="H158" s="2">
         <v>107321458</v>
       </c>
-      <c r="I158" s="5">
+      <c r="I158" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="159" spans="1:9">
+      <c r="J158" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10">
       <c r="A159">
         <v>4739</v>
       </c>
@@ -7297,11 +7592,12 @@
       <c r="H159" s="2">
         <v>107136541</v>
       </c>
-      <c r="I159" s="5">
+      <c r="I159" s="1">
         <v>17750</v>
       </c>
-    </row>
-    <row r="160" spans="1:9">
+      <c r="J159" s="1"/>
+    </row>
+    <row r="160" spans="1:10">
       <c r="A160">
         <v>4787</v>
       </c>
@@ -7326,11 +7622,14 @@
       <c r="H160" s="2">
         <v>106804564</v>
       </c>
-      <c r="I160" s="5">
+      <c r="I160" s="1">
         <v>11430</v>
       </c>
-    </row>
-    <row r="161" spans="1:9">
+      <c r="J160" s="1">
+        <v>11180</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10">
       <c r="A161">
         <v>4842</v>
       </c>
@@ -7355,11 +7654,12 @@
       <c r="H161" s="1">
         <v>0</v>
       </c>
-      <c r="I161" s="5">
+      <c r="I161" s="1">
         <v>12345</v>
       </c>
-    </row>
-    <row r="162" spans="1:9">
+      <c r="J161" s="1"/>
+    </row>
+    <row r="162" spans="1:10">
       <c r="A162">
         <v>4847</v>
       </c>
@@ -7384,11 +7684,14 @@
       <c r="H162" s="1">
         <v>0</v>
       </c>
-      <c r="I162" s="5">
+      <c r="I162" s="1">
         <v>17533</v>
       </c>
-    </row>
-    <row r="163" spans="1:9">
+      <c r="J162" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10">
       <c r="A163">
         <v>4876</v>
       </c>
@@ -7413,11 +7716,12 @@
       <c r="H163" s="2">
         <v>107177994</v>
       </c>
-      <c r="I163" s="5">
+      <c r="I163" s="1">
         <v>17352</v>
       </c>
-    </row>
-    <row r="164" spans="1:9">
+      <c r="J163" s="1"/>
+    </row>
+    <row r="164" spans="1:10">
       <c r="A164">
         <v>4892</v>
       </c>
@@ -7442,11 +7746,12 @@
       <c r="H164" s="2">
         <v>106872681</v>
       </c>
-      <c r="I164" s="5">
+      <c r="I164" s="1">
         <v>17772</v>
       </c>
-    </row>
-    <row r="165" spans="1:9">
+      <c r="J164" s="1"/>
+    </row>
+    <row r="165" spans="1:10">
       <c r="A165">
         <v>4906</v>
       </c>
@@ -7471,11 +7776,14 @@
       <c r="H165" s="1">
         <v>0</v>
       </c>
-      <c r="I165" s="5">
+      <c r="I165" s="1">
         <v>17533</v>
       </c>
-    </row>
-    <row r="166" spans="1:9">
+      <c r="J165" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10">
       <c r="A166">
         <v>4907</v>
       </c>
@@ -7500,11 +7808,12 @@
       <c r="H166" s="2">
         <v>106872681</v>
       </c>
-      <c r="I166" s="5">
+      <c r="I166" s="1">
         <v>16811</v>
       </c>
-    </row>
-    <row r="167" spans="1:9">
+      <c r="J166" s="1"/>
+    </row>
+    <row r="167" spans="1:10">
       <c r="A167">
         <v>4924</v>
       </c>
@@ -7529,11 +7838,12 @@
       <c r="H167" s="1">
         <v>0</v>
       </c>
-      <c r="I167" s="5">
+      <c r="I167" s="1">
         <v>61464</v>
       </c>
-    </row>
-    <row r="168" spans="1:9">
+      <c r="J167" s="1"/>
+    </row>
+    <row r="168" spans="1:10">
       <c r="A168">
         <v>4959</v>
       </c>
@@ -7558,11 +7868,12 @@
       <c r="H168" s="1">
         <v>0</v>
       </c>
-      <c r="I168" s="5">
+      <c r="I168" s="1">
         <v>40277</v>
       </c>
-    </row>
-    <row r="169" spans="1:9">
+      <c r="J168" s="1"/>
+    </row>
+    <row r="169" spans="1:10">
       <c r="A169">
         <v>4976</v>
       </c>
@@ -7587,11 +7898,12 @@
       <c r="H169" s="1">
         <v>0</v>
       </c>
-      <c r="I169" s="5">
+      <c r="I169" s="1">
         <v>40277</v>
       </c>
-    </row>
-    <row r="170" spans="1:9">
+      <c r="J169" s="1"/>
+    </row>
+    <row r="170" spans="1:10">
       <c r="A170">
         <v>4980</v>
       </c>
@@ -7616,11 +7928,12 @@
       <c r="H170" s="2">
         <v>106579602</v>
       </c>
-      <c r="I170" s="5">
+      <c r="I170" s="1">
         <v>15561</v>
       </c>
-    </row>
-    <row r="171" spans="1:9">
+      <c r="J170" s="1"/>
+    </row>
+    <row r="171" spans="1:10">
       <c r="A171">
         <v>5010</v>
       </c>
@@ -7645,11 +7958,12 @@
       <c r="H171" s="1">
         <v>0</v>
       </c>
-      <c r="I171" s="5">
+      <c r="I171" s="1">
         <v>24252</v>
       </c>
-    </row>
-    <row r="172" spans="1:9">
+      <c r="J171" s="1"/>
+    </row>
+    <row r="172" spans="1:10">
       <c r="A172">
         <v>5012</v>
       </c>
@@ -7674,11 +7988,12 @@
       <c r="H172" s="1">
         <v>0</v>
       </c>
-      <c r="I172" s="5">
+      <c r="I172" s="1">
         <v>27685</v>
       </c>
-    </row>
-    <row r="173" spans="1:9">
+      <c r="J172" s="1"/>
+    </row>
+    <row r="173" spans="1:10">
       <c r="A173">
         <v>5013</v>
       </c>
@@ -7703,11 +8018,12 @@
       <c r="H173" s="1">
         <v>0</v>
       </c>
-      <c r="I173" s="5">
+      <c r="I173" s="1">
         <v>28783</v>
       </c>
-    </row>
-    <row r="174" spans="1:9">
+      <c r="J173" s="1"/>
+    </row>
+    <row r="174" spans="1:10">
       <c r="A174">
         <v>5020</v>
       </c>
@@ -7732,11 +8048,12 @@
       <c r="H174" s="1">
         <v>0</v>
       </c>
-      <c r="I174" s="5">
+      <c r="I174" s="1">
         <v>28553</v>
       </c>
-    </row>
-    <row r="175" spans="1:9">
+      <c r="J174" s="1"/>
+    </row>
+    <row r="175" spans="1:10">
       <c r="A175">
         <v>5038</v>
       </c>
@@ -7761,11 +8078,12 @@
       <c r="H175" s="1">
         <v>0</v>
       </c>
-      <c r="I175" s="5">
+      <c r="I175" s="1">
         <v>15721</v>
       </c>
-    </row>
-    <row r="176" spans="1:9">
+      <c r="J175" s="1"/>
+    </row>
+    <row r="176" spans="1:10">
       <c r="A176">
         <v>5054</v>
       </c>
@@ -7790,11 +8108,12 @@
       <c r="H176" s="1">
         <v>0</v>
       </c>
-      <c r="I176" s="5">
+      <c r="I176" s="1">
         <v>41386</v>
       </c>
-    </row>
-    <row r="177" spans="1:9">
+      <c r="J176" s="1"/>
+    </row>
+    <row r="177" spans="1:10">
       <c r="A177">
         <v>5077</v>
       </c>
@@ -7819,11 +8138,12 @@
       <c r="H177" s="1">
         <v>0</v>
       </c>
-      <c r="I177" s="5">
+      <c r="I177" s="1">
         <v>22731</v>
       </c>
-    </row>
-    <row r="178" spans="1:9">
+      <c r="J177" s="1"/>
+    </row>
+    <row r="178" spans="1:10">
       <c r="A178">
         <v>5116</v>
       </c>
@@ -7848,11 +8168,12 @@
       <c r="H178" s="2">
         <v>107177994</v>
       </c>
-      <c r="I178" s="5">
+      <c r="I178" s="1">
         <v>17352</v>
       </c>
-    </row>
-    <row r="179" spans="1:9">
+      <c r="J178" s="1"/>
+    </row>
+    <row r="179" spans="1:10">
       <c r="A179">
         <v>5237</v>
       </c>
@@ -7877,11 +8198,14 @@
       <c r="H179" s="2">
         <v>107121992</v>
       </c>
-      <c r="I179" s="5">
+      <c r="I179" s="1">
         <v>17532</v>
       </c>
-    </row>
-    <row r="180" spans="1:9">
+      <c r="J179" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10">
       <c r="A180">
         <v>5240</v>
       </c>
@@ -7906,11 +8230,12 @@
       <c r="H180" s="1">
         <v>0</v>
       </c>
-      <c r="I180" s="5">
+      <c r="I180" s="1">
         <v>80363</v>
       </c>
-    </row>
-    <row r="181" spans="1:9">
+      <c r="J180" s="1"/>
+    </row>
+    <row r="181" spans="1:10">
       <c r="A181">
         <v>5265</v>
       </c>
@@ -7935,11 +8260,12 @@
       <c r="H181" s="1">
         <v>0</v>
       </c>
-      <c r="I181" s="5">
+      <c r="I181" s="1">
         <v>28783</v>
       </c>
-    </row>
-    <row r="182" spans="1:9">
+      <c r="J181" s="1"/>
+    </row>
+    <row r="182" spans="1:10">
       <c r="A182">
         <v>5267</v>
       </c>
@@ -7964,11 +8290,12 @@
       <c r="H182" s="1">
         <v>0</v>
       </c>
-      <c r="I182" s="5">
+      <c r="I182" s="1">
         <v>20272</v>
       </c>
-    </row>
-    <row r="183" spans="1:9">
+      <c r="J182" s="1"/>
+    </row>
+    <row r="183" spans="1:10">
       <c r="A183">
         <v>5269</v>
       </c>
@@ -7993,11 +8320,12 @@
       <c r="H183" s="1">
         <v>0</v>
       </c>
-      <c r="I183" s="5">
+      <c r="I183" s="1">
         <v>28783</v>
       </c>
-    </row>
-    <row r="184" spans="1:9">
+      <c r="J183" s="1"/>
+    </row>
+    <row r="184" spans="1:10">
       <c r="A184">
         <v>5279</v>
       </c>
@@ -8022,11 +8350,12 @@
       <c r="H184" s="1">
         <v>0</v>
       </c>
-      <c r="I184" s="5">
+      <c r="I184" s="1">
         <v>20272</v>
       </c>
-    </row>
-    <row r="185" spans="1:9">
+      <c r="J184" s="1"/>
+    </row>
+    <row r="185" spans="1:10">
       <c r="A185">
         <v>5280</v>
       </c>
@@ -8051,11 +8380,12 @@
       <c r="H185" s="1">
         <v>0</v>
       </c>
-      <c r="I185" s="5">
+      <c r="I185" s="1">
         <v>28783</v>
       </c>
-    </row>
-    <row r="186" spans="1:9">
+      <c r="J185" s="1"/>
+    </row>
+    <row r="186" spans="1:10">
       <c r="A186">
         <v>5290</v>
       </c>
@@ -8080,11 +8410,12 @@
       <c r="H186" s="1">
         <v>0</v>
       </c>
-      <c r="I186" s="5">
+      <c r="I186" s="1">
         <v>20272</v>
       </c>
-    </row>
-    <row r="187" spans="1:9">
+      <c r="J186" s="1"/>
+    </row>
+    <row r="187" spans="1:10">
       <c r="A187">
         <v>5300</v>
       </c>
@@ -8109,11 +8440,12 @@
       <c r="H187" s="1">
         <v>0</v>
       </c>
-      <c r="I187" s="5">
+      <c r="I187" s="1">
         <v>20272</v>
       </c>
-    </row>
-    <row r="188" spans="1:9">
+      <c r="J187" s="1"/>
+    </row>
+    <row r="188" spans="1:10">
       <c r="A188">
         <v>5311</v>
       </c>
@@ -8138,11 +8470,12 @@
       <c r="H188" s="1">
         <v>0</v>
       </c>
-      <c r="I188" s="5">
+      <c r="I188" s="1">
         <v>20272</v>
       </c>
-    </row>
-    <row r="189" spans="1:9">
+      <c r="J188" s="1"/>
+    </row>
+    <row r="189" spans="1:10">
       <c r="A189">
         <v>5321</v>
       </c>
@@ -8167,11 +8500,12 @@
       <c r="H189" s="1">
         <v>0</v>
       </c>
-      <c r="I189" s="5">
+      <c r="I189" s="1">
         <v>28783</v>
       </c>
-    </row>
-    <row r="190" spans="1:9">
+      <c r="J189" s="1"/>
+    </row>
+    <row r="190" spans="1:10">
       <c r="A190">
         <v>5328</v>
       </c>
@@ -8196,11 +8530,12 @@
       <c r="H190" s="1">
         <v>0</v>
       </c>
-      <c r="I190" s="5">
+      <c r="I190" s="1">
         <v>20272</v>
       </c>
-    </row>
-    <row r="191" spans="1:9">
+      <c r="J190" s="1"/>
+    </row>
+    <row r="191" spans="1:10">
       <c r="A191">
         <v>5345</v>
       </c>
@@ -8225,11 +8560,12 @@
       <c r="H191" s="1">
         <v>0</v>
       </c>
-      <c r="I191" s="5">
+      <c r="I191" s="1">
         <v>20272</v>
       </c>
-    </row>
-    <row r="192" spans="1:9">
+      <c r="J191" s="1"/>
+    </row>
+    <row r="192" spans="1:10">
       <c r="A192">
         <v>5351</v>
       </c>
@@ -8254,11 +8590,12 @@
       <c r="H192" s="1">
         <v>0</v>
       </c>
-      <c r="I192" s="5">
+      <c r="I192" s="1">
         <v>20272</v>
       </c>
-    </row>
-    <row r="193" spans="1:9">
+      <c r="J192" s="1"/>
+    </row>
+    <row r="193" spans="1:10">
       <c r="A193">
         <v>5359</v>
       </c>
@@ -8283,11 +8620,12 @@
       <c r="H193" s="1">
         <v>0</v>
       </c>
-      <c r="I193" s="5">
+      <c r="I193" s="1">
         <v>28673</v>
       </c>
-    </row>
-    <row r="194" spans="1:9">
+      <c r="J193" s="1"/>
+    </row>
+    <row r="194" spans="1:10">
       <c r="A194">
         <v>5369</v>
       </c>
@@ -8312,11 +8650,12 @@
       <c r="H194" s="1">
         <v>0</v>
       </c>
-      <c r="I194" s="5">
+      <c r="I194" s="1">
         <v>20272</v>
       </c>
-    </row>
-    <row r="195" spans="1:9">
+      <c r="J194" s="1"/>
+    </row>
+    <row r="195" spans="1:10">
       <c r="A195">
         <v>5371</v>
       </c>
@@ -8341,11 +8680,12 @@
       <c r="H195" s="1">
         <v>0</v>
       </c>
-      <c r="I195" s="5">
+      <c r="I195" s="1">
         <v>28783</v>
       </c>
-    </row>
-    <row r="196" spans="1:9">
+      <c r="J195" s="1"/>
+    </row>
+    <row r="196" spans="1:10">
       <c r="A196">
         <v>5387</v>
       </c>
@@ -8370,11 +8710,12 @@
       <c r="H196" s="1">
         <v>0</v>
       </c>
-      <c r="I196" s="5">
+      <c r="I196" s="1">
         <v>29668</v>
       </c>
-    </row>
-    <row r="197" spans="1:9">
+      <c r="J196" s="1"/>
+    </row>
+    <row r="197" spans="1:10">
       <c r="A197">
         <v>5391</v>
       </c>
@@ -8399,11 +8740,14 @@
       <c r="H197" s="1">
         <v>0</v>
       </c>
-      <c r="I197" s="5">
+      <c r="I197" s="1">
         <v>17532</v>
       </c>
-    </row>
-    <row r="198" spans="1:9">
+      <c r="J197" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10">
       <c r="A198">
         <v>5413</v>
       </c>
@@ -8428,11 +8772,12 @@
       <c r="H198" s="1">
         <v>0</v>
       </c>
-      <c r="I198" s="5">
+      <c r="I198" s="1">
         <v>21169</v>
       </c>
-    </row>
-    <row r="199" spans="1:9">
+      <c r="J198" s="1"/>
+    </row>
+    <row r="199" spans="1:10">
       <c r="A199">
         <v>5460</v>
       </c>
@@ -8457,11 +8802,12 @@
       <c r="H199" s="1">
         <v>0</v>
       </c>
-      <c r="I199" s="5">
+      <c r="I199" s="1">
         <v>28637</v>
       </c>
-    </row>
-    <row r="200" spans="1:9">
+      <c r="J199" s="1"/>
+    </row>
+    <row r="200" spans="1:10">
       <c r="A200">
         <v>5463</v>
       </c>
@@ -8486,11 +8832,12 @@
       <c r="H200" s="1">
         <v>0</v>
       </c>
-      <c r="I200" s="5">
+      <c r="I200" s="1">
         <v>26455</v>
       </c>
-    </row>
-    <row r="201" spans="1:9">
+      <c r="J200" s="1"/>
+    </row>
+    <row r="201" spans="1:10">
       <c r="A201">
         <v>5496</v>
       </c>
@@ -8515,11 +8862,12 @@
       <c r="H201" s="2">
         <v>106579602</v>
       </c>
-      <c r="I201" s="5">
+      <c r="I201" s="1">
         <v>15561</v>
       </c>
-    </row>
-    <row r="202" spans="1:9">
+      <c r="J201" s="1"/>
+    </row>
+    <row r="202" spans="1:10">
       <c r="A202">
         <v>5510</v>
       </c>
@@ -8544,11 +8892,12 @@
       <c r="H202" s="2">
         <v>99161808</v>
       </c>
-      <c r="I202" s="5">
+      <c r="I202" s="1">
         <v>20999</v>
       </c>
-    </row>
-    <row r="203" spans="1:9">
+      <c r="J202" s="1"/>
+    </row>
+    <row r="203" spans="1:10">
       <c r="A203">
         <v>5511</v>
       </c>
@@ -8573,11 +8922,12 @@
       <c r="H203" s="1">
         <v>0</v>
       </c>
-      <c r="I203" s="5">
+      <c r="I203" s="1">
         <v>22277</v>
       </c>
-    </row>
-    <row r="204" spans="1:9">
+      <c r="J203" s="1"/>
+    </row>
+    <row r="204" spans="1:10">
       <c r="A204">
         <v>5517</v>
       </c>
@@ -8602,11 +8952,12 @@
       <c r="H204" s="1">
         <v>0</v>
       </c>
-      <c r="I204" s="5">
+      <c r="I204" s="1">
         <v>28783</v>
       </c>
-    </row>
-    <row r="205" spans="1:9">
+      <c r="J204" s="1"/>
+    </row>
+    <row r="205" spans="1:10">
       <c r="A205">
         <v>5522</v>
       </c>
@@ -8631,11 +8982,12 @@
       <c r="H205" s="1">
         <v>0</v>
       </c>
-      <c r="I205" s="5">
+      <c r="I205" s="1">
         <v>29358</v>
       </c>
-    </row>
-    <row r="206" spans="1:9">
+      <c r="J205" s="1"/>
+    </row>
+    <row r="206" spans="1:10">
       <c r="A206">
         <v>5524</v>
       </c>
@@ -8660,11 +9012,12 @@
       <c r="H206" s="2">
         <v>110701295</v>
       </c>
-      <c r="I206" s="5">
+      <c r="I206" s="1">
         <v>59460</v>
       </c>
-    </row>
-    <row r="207" spans="1:9">
+      <c r="J206" s="1"/>
+    </row>
+    <row r="207" spans="1:10">
       <c r="A207">
         <v>5530</v>
       </c>
@@ -8689,11 +9042,14 @@
       <c r="H207" s="2">
         <v>107321461</v>
       </c>
-      <c r="I207" s="5">
+      <c r="I207" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="208" spans="1:9">
+      <c r="J207" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10">
       <c r="A208">
         <v>5533</v>
       </c>
@@ -8718,11 +9074,12 @@
       <c r="H208" s="1">
         <v>0</v>
       </c>
-      <c r="I208" s="5">
+      <c r="I208" s="1">
         <v>57523</v>
       </c>
-    </row>
-    <row r="209" spans="1:9">
+      <c r="J208" s="1"/>
+    </row>
+    <row r="209" spans="1:10">
       <c r="A209">
         <v>5548</v>
       </c>
@@ -8747,11 +9104,14 @@
       <c r="H209" s="2">
         <v>107321458</v>
       </c>
-      <c r="I209" s="5">
+      <c r="I209" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="210" spans="1:9">
+      <c r="J209" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10">
       <c r="A210">
         <v>5567</v>
       </c>
@@ -8776,11 +9136,12 @@
       <c r="H210" s="1">
         <v>0</v>
       </c>
-      <c r="I210" s="5">
+      <c r="I210" s="1">
         <v>41386</v>
       </c>
-    </row>
-    <row r="211" spans="1:9">
+      <c r="J210" s="1"/>
+    </row>
+    <row r="211" spans="1:10">
       <c r="A211">
         <v>5600</v>
       </c>
@@ -8805,11 +9166,12 @@
       <c r="H211" s="1">
         <v>0</v>
       </c>
-      <c r="I211" s="5">
+      <c r="I211" s="1">
         <v>28783</v>
       </c>
-    </row>
-    <row r="212" spans="1:9">
+      <c r="J211" s="1"/>
+    </row>
+    <row r="212" spans="1:10">
       <c r="A212">
         <v>5641</v>
       </c>
@@ -8834,11 +9196,12 @@
       <c r="H212" s="1">
         <v>0</v>
       </c>
-      <c r="I212" s="5">
+      <c r="I212" s="1">
         <v>28783</v>
       </c>
-    </row>
-    <row r="213" spans="1:9">
+      <c r="J212" s="1"/>
+    </row>
+    <row r="213" spans="1:10">
       <c r="A213">
         <v>5648</v>
       </c>
@@ -8863,11 +9226,12 @@
       <c r="H213" s="1">
         <v>0</v>
       </c>
-      <c r="I213" s="5">
+      <c r="I213" s="1">
         <v>20272</v>
       </c>
-    </row>
-    <row r="214" spans="1:9">
+      <c r="J213" s="1"/>
+    </row>
+    <row r="214" spans="1:10">
       <c r="A214">
         <v>5650</v>
       </c>
@@ -8892,11 +9256,12 @@
       <c r="H214" s="1">
         <v>0</v>
       </c>
-      <c r="I214" s="5">
+      <c r="I214" s="1">
         <v>28783</v>
       </c>
-    </row>
-    <row r="215" spans="1:9">
+      <c r="J214" s="1"/>
+    </row>
+    <row r="215" spans="1:10">
       <c r="A215">
         <v>5660</v>
       </c>
@@ -8921,11 +9286,14 @@
       <c r="H215" s="2">
         <v>107321461</v>
       </c>
-      <c r="I215" s="5">
+      <c r="I215" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="216" spans="1:9">
+      <c r="J215" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10">
       <c r="A216">
         <v>5668</v>
       </c>
@@ -8950,11 +9318,12 @@
       <c r="H216" s="2">
         <v>107471637</v>
       </c>
-      <c r="I216" s="5">
+      <c r="I216" s="1">
         <v>41376</v>
       </c>
-    </row>
-    <row r="217" spans="1:9">
+      <c r="J216" s="1"/>
+    </row>
+    <row r="217" spans="1:10">
       <c r="A217">
         <v>5677</v>
       </c>
@@ -8979,11 +9348,12 @@
       <c r="H217" s="1">
         <v>0</v>
       </c>
-      <c r="I217" s="5">
+      <c r="I217" s="1">
         <v>20272</v>
       </c>
-    </row>
-    <row r="218" spans="1:9">
+      <c r="J217" s="1"/>
+    </row>
+    <row r="218" spans="1:10">
       <c r="A218">
         <v>5680</v>
       </c>
@@ -9008,11 +9378,12 @@
       <c r="H218" s="1">
         <v>0</v>
       </c>
-      <c r="I218" s="5">
+      <c r="I218" s="1">
         <v>28783</v>
       </c>
-    </row>
-    <row r="219" spans="1:9">
+      <c r="J218" s="1"/>
+    </row>
+    <row r="219" spans="1:10">
       <c r="A219">
         <v>5694</v>
       </c>
@@ -9037,11 +9408,12 @@
       <c r="H219" s="1">
         <v>0</v>
       </c>
-      <c r="I219" s="5">
+      <c r="I219" s="1">
         <v>20272</v>
       </c>
-    </row>
-    <row r="220" spans="1:9">
+      <c r="J219" s="1"/>
+    </row>
+    <row r="220" spans="1:10">
       <c r="A220">
         <v>5697</v>
       </c>
@@ -9066,11 +9438,12 @@
       <c r="H220" s="1">
         <v>0</v>
       </c>
-      <c r="I220" s="5">
+      <c r="I220" s="1">
         <v>28783</v>
       </c>
-    </row>
-    <row r="221" spans="1:9">
+      <c r="J220" s="1"/>
+    </row>
+    <row r="221" spans="1:10">
       <c r="A221">
         <v>5783</v>
       </c>
@@ -9095,11 +9468,12 @@
       <c r="H221" s="2">
         <v>107680431</v>
       </c>
-      <c r="I221" s="5">
+      <c r="I221" s="1">
         <v>40296</v>
       </c>
-    </row>
-    <row r="222" spans="1:9">
+      <c r="J221" s="1"/>
+    </row>
+    <row r="222" spans="1:10">
       <c r="A222">
         <v>5832</v>
       </c>
@@ -9124,11 +9498,12 @@
       <c r="H222" s="2">
         <v>107680431</v>
       </c>
-      <c r="I222" s="5">
+      <c r="I222" s="1">
         <v>40296</v>
       </c>
-    </row>
-    <row r="223" spans="1:9">
+      <c r="J222" s="1"/>
+    </row>
+    <row r="223" spans="1:10">
       <c r="A223">
         <v>5984</v>
       </c>
@@ -9153,11 +9528,12 @@
       <c r="H223" s="1">
         <v>0</v>
       </c>
-      <c r="I223" s="5">
+      <c r="I223" s="1">
         <v>28783</v>
       </c>
-    </row>
-    <row r="224" spans="1:9">
+      <c r="J223" s="1"/>
+    </row>
+    <row r="224" spans="1:10">
       <c r="A224">
         <v>5992</v>
       </c>
@@ -9182,11 +9558,12 @@
       <c r="H224" s="1">
         <v>0</v>
       </c>
-      <c r="I224" s="5">
+      <c r="I224" s="1">
         <v>80363</v>
       </c>
-    </row>
-    <row r="225" spans="1:9">
+      <c r="J224" s="1"/>
+    </row>
+    <row r="225" spans="1:10">
       <c r="A225">
         <v>5996</v>
       </c>
@@ -9211,11 +9588,12 @@
       <c r="H225" s="2">
         <v>106579602</v>
       </c>
-      <c r="I225" s="5">
+      <c r="I225" s="1">
         <v>15561</v>
       </c>
-    </row>
-    <row r="226" spans="1:9">
+      <c r="J225" s="1"/>
+    </row>
+    <row r="226" spans="1:10">
       <c r="A226">
         <v>6021</v>
       </c>
@@ -9240,11 +9618,12 @@
       <c r="H226" s="2">
         <v>107136541</v>
       </c>
-      <c r="I226" s="5">
+      <c r="I226" s="1">
         <v>17750</v>
       </c>
-    </row>
-    <row r="227" spans="1:9">
+      <c r="J226" s="1"/>
+    </row>
+    <row r="227" spans="1:10">
       <c r="A227">
         <v>6032</v>
       </c>
@@ -9269,11 +9648,14 @@
       <c r="H227" s="1">
         <v>0</v>
       </c>
-      <c r="I227" s="5">
+      <c r="I227" s="1">
         <v>17533</v>
       </c>
-    </row>
-    <row r="228" spans="1:9">
+      <c r="J227" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10">
       <c r="A228">
         <v>6064</v>
       </c>
@@ -9298,11 +9680,14 @@
       <c r="H228" s="2">
         <v>106804564</v>
       </c>
-      <c r="I228" s="5">
+      <c r="I228" s="1">
         <v>11430</v>
       </c>
-    </row>
-    <row r="229" spans="1:9">
+      <c r="J228" s="1">
+        <v>11180</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10">
       <c r="A229">
         <v>6091</v>
       </c>
@@ -9327,11 +9712,14 @@
       <c r="H229" s="2">
         <v>107321461</v>
       </c>
-      <c r="I229" s="5">
+      <c r="I229" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="230" spans="1:9">
+      <c r="J229" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10">
       <c r="A230">
         <v>6152</v>
       </c>
@@ -9356,11 +9744,12 @@
       <c r="H230" s="2">
         <v>107177994</v>
       </c>
-      <c r="I230" s="5">
+      <c r="I230" s="1">
         <v>17352</v>
       </c>
-    </row>
-    <row r="231" spans="1:9">
+      <c r="J230" s="1"/>
+    </row>
+    <row r="231" spans="1:10">
       <c r="A231">
         <v>6179</v>
       </c>
@@ -9385,11 +9774,14 @@
       <c r="H231" s="2">
         <v>106804564</v>
       </c>
-      <c r="I231" s="5">
+      <c r="I231" s="1">
         <v>11430</v>
       </c>
-    </row>
-    <row r="232" spans="1:9">
+      <c r="J231" s="1">
+        <v>11180</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10">
       <c r="A232">
         <v>6202</v>
       </c>
@@ -9414,11 +9806,12 @@
       <c r="H232" s="1">
         <v>0</v>
       </c>
-      <c r="I232" s="5">
+      <c r="I232" s="1">
         <v>20272</v>
       </c>
-    </row>
-    <row r="233" spans="1:9">
+      <c r="J232" s="1"/>
+    </row>
+    <row r="233" spans="1:10">
       <c r="A233">
         <v>6211</v>
       </c>
@@ -9443,11 +9836,12 @@
       <c r="H233" s="1">
         <v>0</v>
       </c>
-      <c r="I233" s="5">
+      <c r="I233" s="1">
         <v>57523</v>
       </c>
-    </row>
-    <row r="234" spans="1:9">
+      <c r="J233" s="1"/>
+    </row>
+    <row r="234" spans="1:10">
       <c r="A234">
         <v>6219</v>
       </c>
@@ -9472,11 +9866,12 @@
       <c r="H234" s="1">
         <v>0</v>
       </c>
-      <c r="I234" s="5">
+      <c r="I234" s="1">
         <v>41376</v>
       </c>
-    </row>
-    <row r="235" spans="1:9">
+      <c r="J234" s="1"/>
+    </row>
+    <row r="235" spans="1:10">
       <c r="A235">
         <v>6221</v>
       </c>
@@ -9501,11 +9896,12 @@
       <c r="H235" s="2">
         <v>107680431</v>
       </c>
-      <c r="I235" s="5">
+      <c r="I235" s="1">
         <v>40296</v>
       </c>
-    </row>
-    <row r="236" spans="1:9">
+      <c r="J235" s="1"/>
+    </row>
+    <row r="236" spans="1:10">
       <c r="A236">
         <v>6299</v>
       </c>
@@ -9530,11 +9926,12 @@
       <c r="H236" s="2">
         <v>10137646</v>
       </c>
-      <c r="I236" s="5">
+      <c r="I236" s="1">
         <v>28296</v>
       </c>
-    </row>
-    <row r="237" spans="1:9">
+      <c r="J236" s="1"/>
+    </row>
+    <row r="237" spans="1:10">
       <c r="A237">
         <v>6370</v>
       </c>
@@ -9559,11 +9956,12 @@
       <c r="H237" s="2">
         <v>110986694</v>
       </c>
-      <c r="I237" s="5">
+      <c r="I237" s="1">
         <v>57771</v>
       </c>
-    </row>
-    <row r="238" spans="1:9">
+      <c r="J237" s="1"/>
+    </row>
+    <row r="238" spans="1:10">
       <c r="A238">
         <v>6375</v>
       </c>
@@ -9588,11 +9986,12 @@
       <c r="H238" s="1">
         <v>0</v>
       </c>
-      <c r="I238" s="5">
+      <c r="I238" s="1">
         <v>28783</v>
       </c>
-    </row>
-    <row r="239" spans="1:9">
+      <c r="J238" s="1"/>
+    </row>
+    <row r="239" spans="1:10">
       <c r="A239">
         <v>6400</v>
       </c>
@@ -9617,11 +10016,12 @@
       <c r="H239" s="1">
         <v>0</v>
       </c>
-      <c r="I239" s="5">
+      <c r="I239" s="1">
         <v>20272</v>
       </c>
-    </row>
-    <row r="240" spans="1:9">
+      <c r="J239" s="1"/>
+    </row>
+    <row r="240" spans="1:10">
       <c r="A240">
         <v>6414</v>
       </c>
@@ -9646,11 +10046,14 @@
       <c r="H240" s="2">
         <v>107478382</v>
       </c>
-      <c r="I240" s="5">
+      <c r="I240" s="1">
         <v>40714</v>
       </c>
-    </row>
-    <row r="241" spans="1:9">
+      <c r="J240" s="1">
+        <v>40553</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10">
       <c r="A241">
         <v>6433</v>
       </c>
@@ -9675,11 +10078,12 @@
       <c r="H241" s="1">
         <v>0</v>
       </c>
-      <c r="I241" s="5">
+      <c r="I241" s="1">
         <v>30761</v>
       </c>
-    </row>
-    <row r="242" spans="1:9">
+      <c r="J241" s="1"/>
+    </row>
+    <row r="242" spans="1:10">
       <c r="A242">
         <v>6458</v>
       </c>
@@ -9704,11 +10108,14 @@
       <c r="H242" s="2">
         <v>107121992</v>
       </c>
-      <c r="I242" s="5">
+      <c r="I242" s="1">
         <v>17532</v>
       </c>
-    </row>
-    <row r="243" spans="1:9">
+      <c r="J242" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="243" spans="1:10">
       <c r="A243">
         <v>6462</v>
       </c>
@@ -9733,11 +10140,12 @@
       <c r="H243" s="2">
         <v>98947144</v>
       </c>
-      <c r="I243" s="5">
+      <c r="I243" s="1">
         <v>20985</v>
       </c>
-    </row>
-    <row r="244" spans="1:9">
+      <c r="J243" s="1"/>
+    </row>
+    <row r="244" spans="1:10">
       <c r="A244">
         <v>6494</v>
       </c>
@@ -9762,11 +10170,12 @@
       <c r="H244" s="1">
         <v>0</v>
       </c>
-      <c r="I244" s="5">
+      <c r="I244" s="1">
         <v>41376</v>
       </c>
-    </row>
-    <row r="245" spans="1:9">
+      <c r="J244" s="1"/>
+    </row>
+    <row r="245" spans="1:10">
       <c r="A245">
         <v>6517</v>
       </c>
@@ -9791,11 +10200,12 @@
       <c r="H245" s="1">
         <v>0</v>
       </c>
-      <c r="I245" s="5">
+      <c r="I245" s="1">
         <v>61131</v>
       </c>
-    </row>
-    <row r="246" spans="1:9">
+      <c r="J245" s="1"/>
+    </row>
+    <row r="246" spans="1:10">
       <c r="A246">
         <v>6588</v>
       </c>
@@ -9820,11 +10230,12 @@
       <c r="H246" s="1">
         <v>0</v>
       </c>
-      <c r="I246" s="5">
+      <c r="I246" s="1">
         <v>16611</v>
       </c>
-    </row>
-    <row r="247" spans="1:9">
+      <c r="J246" s="1"/>
+    </row>
+    <row r="247" spans="1:10">
       <c r="A247">
         <v>6605</v>
       </c>
@@ -9849,11 +10260,12 @@
       <c r="H247" s="2">
         <v>106678458</v>
       </c>
-      <c r="I247" s="5">
+      <c r="I247" s="1">
         <v>19110</v>
       </c>
-    </row>
-    <row r="248" spans="1:9">
+      <c r="J247" s="1"/>
+    </row>
+    <row r="248" spans="1:10">
       <c r="A248">
         <v>6651</v>
       </c>
@@ -9878,11 +10290,14 @@
       <c r="H248" s="2">
         <v>107121992</v>
       </c>
-      <c r="I248" s="5">
+      <c r="I248" s="1">
         <v>17532</v>
       </c>
-    </row>
-    <row r="249" spans="1:9">
+      <c r="J248" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="249" spans="1:10">
       <c r="A249">
         <v>6662</v>
       </c>
@@ -9907,11 +10322,14 @@
       <c r="H249" s="2">
         <v>107321461</v>
       </c>
-      <c r="I249" s="5">
+      <c r="I249" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="250" spans="1:9">
+      <c r="J249" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10">
       <c r="A250">
         <v>6750</v>
       </c>
@@ -9936,11 +10354,12 @@
       <c r="H250" s="2">
         <v>107320233</v>
       </c>
-      <c r="I250" s="5">
+      <c r="I250" s="1">
         <v>41326</v>
       </c>
-    </row>
-    <row r="251" spans="1:9">
+      <c r="J250" s="1"/>
+    </row>
+    <row r="251" spans="1:10">
       <c r="A251">
         <v>6801</v>
       </c>
@@ -9965,11 +10384,12 @@
       <c r="H251" s="1">
         <v>0</v>
       </c>
-      <c r="I251" s="5">
+      <c r="I251" s="1">
         <v>17450</v>
       </c>
-    </row>
-    <row r="252" spans="1:9">
+      <c r="J251" s="1"/>
+    </row>
+    <row r="252" spans="1:10">
       <c r="A252">
         <v>6830</v>
       </c>
@@ -9994,11 +10414,12 @@
       <c r="H252" s="1">
         <v>0</v>
       </c>
-      <c r="I252" s="5">
+      <c r="I252" s="1">
         <v>17450</v>
       </c>
-    </row>
-    <row r="253" spans="1:9">
+      <c r="J252" s="1"/>
+    </row>
+    <row r="253" spans="1:10">
       <c r="A253">
         <v>6836</v>
       </c>
@@ -10023,11 +10444,14 @@
       <c r="H253" s="2">
         <v>107121992</v>
       </c>
-      <c r="I253" s="5">
+      <c r="I253" s="1">
         <v>17532</v>
       </c>
-    </row>
-    <row r="254" spans="1:9">
+      <c r="J253" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="254" spans="1:10">
       <c r="A254">
         <v>6848</v>
       </c>
@@ -10052,11 +10476,12 @@
       <c r="H254" s="2">
         <v>106900555</v>
       </c>
-      <c r="I254" s="5">
+      <c r="I254" s="1">
         <v>16811</v>
       </c>
-    </row>
-    <row r="255" spans="1:9">
+      <c r="J254" s="1"/>
+    </row>
+    <row r="255" spans="1:10">
       <c r="A255">
         <v>6866</v>
       </c>
@@ -10081,11 +10506,14 @@
       <c r="H255" s="2">
         <v>107187905</v>
       </c>
-      <c r="I255" s="5">
+      <c r="I255" s="1">
         <v>17533</v>
       </c>
-    </row>
-    <row r="256" spans="1:9">
+      <c r="J255" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10">
       <c r="A256">
         <v>6880</v>
       </c>
@@ -10110,11 +10538,12 @@
       <c r="H256" s="1">
         <v>0</v>
       </c>
-      <c r="I256" s="5">
+      <c r="I256" s="1">
         <v>17450</v>
       </c>
-    </row>
-    <row r="257" spans="1:9">
+      <c r="J256" s="1"/>
+    </row>
+    <row r="257" spans="1:10">
       <c r="A257">
         <v>6965</v>
       </c>
@@ -10139,11 +10568,12 @@
       <c r="H257" s="1">
         <v>0</v>
       </c>
-      <c r="I257" s="5">
+      <c r="I257" s="1">
         <v>21276</v>
       </c>
-    </row>
-    <row r="258" spans="1:9">
+      <c r="J257" s="1"/>
+    </row>
+    <row r="258" spans="1:10">
       <c r="A258">
         <v>7027</v>
       </c>
@@ -10168,11 +10598,14 @@
       <c r="H258" s="2">
         <v>107121992</v>
       </c>
-      <c r="I258" s="5">
+      <c r="I258" s="1">
         <v>17532</v>
       </c>
-    </row>
-    <row r="259" spans="1:9">
+      <c r="J258" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10">
       <c r="A259">
         <v>7056</v>
       </c>
@@ -10197,11 +10630,14 @@
       <c r="H259" s="2">
         <v>107321461</v>
       </c>
-      <c r="I259" s="5">
+      <c r="I259" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="260" spans="1:9">
+      <c r="J259" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10">
       <c r="A260">
         <v>7155</v>
       </c>
@@ -10226,11 +10662,12 @@
       <c r="H260" s="2">
         <v>10137646</v>
       </c>
-      <c r="I260" s="5">
+      <c r="I260" s="1">
         <v>28296</v>
       </c>
-    </row>
-    <row r="261" spans="1:9">
+      <c r="J260" s="1"/>
+    </row>
+    <row r="261" spans="1:10">
       <c r="A261">
         <v>7173</v>
       </c>
@@ -10255,11 +10692,12 @@
       <c r="H261" s="2">
         <v>10137646</v>
       </c>
-      <c r="I261" s="5">
+      <c r="I261" s="1">
         <v>28296</v>
       </c>
-    </row>
-    <row r="262" spans="1:9">
+      <c r="J261" s="1"/>
+    </row>
+    <row r="262" spans="1:10">
       <c r="A262">
         <v>7198</v>
       </c>
@@ -10284,11 +10722,12 @@
       <c r="H262" s="1">
         <v>0</v>
       </c>
-      <c r="I262" s="5">
+      <c r="I262" s="1">
         <v>45159</v>
       </c>
-    </row>
-    <row r="263" spans="1:9">
+      <c r="J262" s="1"/>
+    </row>
+    <row r="263" spans="1:10">
       <c r="A263">
         <v>7225</v>
       </c>
@@ -10313,11 +10752,14 @@
       <c r="H263" s="1">
         <v>0</v>
       </c>
-      <c r="I263" s="5">
+      <c r="I263" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="264" spans="1:9">
+      <c r="J263" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10">
       <c r="A264">
         <v>7299</v>
       </c>
@@ -10342,11 +10784,14 @@
       <c r="H264" s="1">
         <v>0</v>
       </c>
-      <c r="I264" s="5">
+      <c r="I264" s="1">
         <v>43260</v>
       </c>
-    </row>
-    <row r="265" spans="1:9">
+      <c r="J264" s="1">
+        <v>43261</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10">
       <c r="A265">
         <v>7300</v>
       </c>
@@ -10371,11 +10816,14 @@
       <c r="H265" s="2">
         <v>107321461</v>
       </c>
-      <c r="I265" s="5">
+      <c r="I265" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="266" spans="1:9">
+      <c r="J265" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="266" spans="1:10">
       <c r="A266">
         <v>7321</v>
       </c>
@@ -10400,11 +10848,12 @@
       <c r="H266" s="2">
         <v>106900555</v>
       </c>
-      <c r="I266" s="5">
+      <c r="I266" s="1">
         <v>16811</v>
       </c>
-    </row>
-    <row r="267" spans="1:9">
+      <c r="J266" s="1"/>
+    </row>
+    <row r="267" spans="1:10">
       <c r="A267">
         <v>7325</v>
       </c>
@@ -10429,11 +10878,12 @@
       <c r="H267" s="1">
         <v>0</v>
       </c>
-      <c r="I267" s="5">
+      <c r="I267" s="1">
         <v>21160</v>
       </c>
-    </row>
-    <row r="268" spans="1:9">
+      <c r="J267" s="1"/>
+    </row>
+    <row r="268" spans="1:10">
       <c r="A268">
         <v>7417</v>
       </c>
@@ -10458,11 +10908,12 @@
       <c r="H268" s="2">
         <v>106900555</v>
       </c>
-      <c r="I268" s="5">
+      <c r="I268" s="1">
         <v>16811</v>
       </c>
-    </row>
-    <row r="269" spans="1:9">
+      <c r="J268" s="1"/>
+    </row>
+    <row r="269" spans="1:10">
       <c r="A269">
         <v>7433</v>
       </c>
@@ -10487,11 +10938,14 @@
       <c r="H269" s="2">
         <v>107321461</v>
       </c>
-      <c r="I269" s="5">
+      <c r="I269" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="270" spans="1:9">
+      <c r="J269" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="270" spans="1:10">
       <c r="A270">
         <v>7442</v>
       </c>
@@ -10516,11 +10970,12 @@
       <c r="H270" s="1">
         <v>0</v>
       </c>
-      <c r="I270" s="5">
+      <c r="I270" s="1">
         <v>42421</v>
       </c>
-    </row>
-    <row r="271" spans="1:9">
+      <c r="J270" s="1"/>
+    </row>
+    <row r="271" spans="1:10">
       <c r="A271">
         <v>7449</v>
       </c>
@@ -10545,11 +11000,12 @@
       <c r="H271" s="2">
         <v>107680431</v>
       </c>
-      <c r="I271" s="5">
+      <c r="I271" s="1">
         <v>40296</v>
       </c>
-    </row>
-    <row r="272" spans="1:9">
+      <c r="J271" s="1"/>
+    </row>
+    <row r="272" spans="1:10">
       <c r="A272">
         <v>7477</v>
       </c>
@@ -10574,11 +11030,14 @@
       <c r="H272" s="2">
         <v>107121992</v>
       </c>
-      <c r="I272" s="5">
+      <c r="I272" s="1">
         <v>17532</v>
       </c>
-    </row>
-    <row r="273" spans="1:9">
+      <c r="J272" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="273" spans="1:10">
       <c r="A273">
         <v>7536</v>
       </c>
@@ -10603,11 +11062,12 @@
       <c r="H273" s="1">
         <v>0</v>
       </c>
-      <c r="I273" s="5">
+      <c r="I273" s="1">
         <v>45159</v>
       </c>
-    </row>
-    <row r="274" spans="1:9">
+      <c r="J273" s="1"/>
+    </row>
+    <row r="274" spans="1:10">
       <c r="A274">
         <v>7539</v>
       </c>
@@ -10632,11 +11092,12 @@
       <c r="H274" s="2">
         <v>99273015</v>
       </c>
-      <c r="I274" s="5">
+      <c r="I274" s="1">
         <v>22730</v>
       </c>
-    </row>
-    <row r="275" spans="1:9">
+      <c r="J274" s="1"/>
+    </row>
+    <row r="275" spans="1:10">
       <c r="A275">
         <v>7565</v>
       </c>
@@ -10661,11 +11122,12 @@
       <c r="H275" s="1">
         <v>0</v>
       </c>
-      <c r="I275" s="5">
+      <c r="I275" s="1">
         <v>34694</v>
       </c>
-    </row>
-    <row r="276" spans="1:9">
+      <c r="J275" s="1"/>
+    </row>
+    <row r="276" spans="1:10">
       <c r="A276">
         <v>7613</v>
       </c>
@@ -10690,11 +11152,12 @@
       <c r="H276" s="1">
         <v>0</v>
       </c>
-      <c r="I276" s="5">
+      <c r="I276" s="1">
         <v>20776</v>
       </c>
-    </row>
-    <row r="277" spans="1:9">
+      <c r="J276" s="1"/>
+    </row>
+    <row r="277" spans="1:10">
       <c r="A277">
         <v>7711</v>
       </c>
@@ -10719,11 +11182,12 @@
       <c r="H277" s="2">
         <v>106900555</v>
       </c>
-      <c r="I277" s="5">
+      <c r="I277" s="1">
         <v>16811</v>
       </c>
-    </row>
-    <row r="278" spans="1:9">
+      <c r="J277" s="1"/>
+    </row>
+    <row r="278" spans="1:10">
       <c r="A278">
         <v>7850</v>
       </c>
@@ -10748,11 +11212,12 @@
       <c r="H278" s="1">
         <v>0</v>
       </c>
-      <c r="I278" s="5">
+      <c r="I278" s="1">
         <v>28783</v>
       </c>
-    </row>
-    <row r="279" spans="1:9">
+      <c r="J278" s="1"/>
+    </row>
+    <row r="279" spans="1:10">
       <c r="A279">
         <v>7862</v>
       </c>
@@ -10777,11 +11242,12 @@
       <c r="H279" s="2">
         <v>107471637</v>
       </c>
-      <c r="I279" s="5">
+      <c r="I279" s="1">
         <v>41376</v>
       </c>
-    </row>
-    <row r="280" spans="1:9">
+      <c r="J279" s="1"/>
+    </row>
+    <row r="280" spans="1:10">
       <c r="A280">
         <v>7863</v>
       </c>
@@ -10806,11 +11272,12 @@
       <c r="H280" s="1">
         <v>0</v>
       </c>
-      <c r="I280" s="5">
+      <c r="I280" s="1">
         <v>21277</v>
       </c>
-    </row>
-    <row r="281" spans="1:9">
+      <c r="J280" s="1"/>
+    </row>
+    <row r="281" spans="1:10">
       <c r="A281">
         <v>7869</v>
       </c>
@@ -10835,11 +11302,12 @@
       <c r="H281" s="2">
         <v>106773595</v>
       </c>
-      <c r="I281" s="5">
+      <c r="I281" s="1">
         <v>51157</v>
       </c>
-    </row>
-    <row r="282" spans="1:9">
+      <c r="J281" s="1"/>
+    </row>
+    <row r="282" spans="1:10">
       <c r="A282">
         <v>7913</v>
       </c>
@@ -10864,11 +11332,12 @@
       <c r="H282" s="1">
         <v>0</v>
       </c>
-      <c r="I282" s="5">
+      <c r="I282" s="1">
         <v>41180</v>
       </c>
-    </row>
-    <row r="283" spans="1:9">
+      <c r="J282" s="1"/>
+    </row>
+    <row r="283" spans="1:10">
       <c r="A283">
         <v>7921</v>
       </c>
@@ -10893,11 +11362,14 @@
       <c r="H283" s="2">
         <v>107321461</v>
       </c>
-      <c r="I283" s="5">
+      <c r="I283" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="284" spans="1:9">
+      <c r="J283" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="284" spans="1:10">
       <c r="A284">
         <v>7978</v>
       </c>
@@ -10922,11 +11394,14 @@
       <c r="H284" s="2">
         <v>107121992</v>
       </c>
-      <c r="I284" s="5">
+      <c r="I284" s="1">
         <v>17532</v>
       </c>
-    </row>
-    <row r="285" spans="1:9">
+      <c r="J284" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="285" spans="1:10">
       <c r="A285">
         <v>7982</v>
       </c>
@@ -10951,11 +11426,12 @@
       <c r="H285" s="2">
         <v>106900555</v>
       </c>
-      <c r="I285" s="5">
+      <c r="I285" s="1">
         <v>16811</v>
       </c>
-    </row>
-    <row r="286" spans="1:9">
+      <c r="J285" s="1"/>
+    </row>
+    <row r="286" spans="1:10">
       <c r="A286">
         <v>8001</v>
       </c>
@@ -10980,11 +11456,12 @@
       <c r="H286" s="1">
         <v>0</v>
       </c>
-      <c r="I286" s="5">
+      <c r="I286" s="1">
         <v>37317</v>
       </c>
-    </row>
-    <row r="287" spans="1:9">
+      <c r="J286" s="1"/>
+    </row>
+    <row r="287" spans="1:10">
       <c r="A287">
         <v>8003</v>
       </c>
@@ -11009,11 +11486,14 @@
       <c r="H287" s="1">
         <v>0</v>
       </c>
-      <c r="I287" s="5">
+      <c r="I287" s="1">
         <v>17532</v>
       </c>
-    </row>
-    <row r="288" spans="1:9">
+      <c r="J287" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="288" spans="1:10">
       <c r="A288">
         <v>8112</v>
       </c>
@@ -11038,11 +11518,14 @@
       <c r="H288" s="2">
         <v>107121992</v>
       </c>
-      <c r="I288" s="5">
+      <c r="I288" s="1">
         <v>17532</v>
       </c>
-    </row>
-    <row r="289" spans="1:9">
+      <c r="J288" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10">
       <c r="A289">
         <v>8113</v>
       </c>
@@ -11067,11 +11550,12 @@
       <c r="H289" s="1">
         <v>0</v>
       </c>
-      <c r="I289" s="5">
+      <c r="I289" s="1">
         <v>15611</v>
       </c>
-    </row>
-    <row r="290" spans="1:9">
+      <c r="J289" s="1"/>
+    </row>
+    <row r="290" spans="1:10">
       <c r="A290">
         <v>8229</v>
       </c>
@@ -11096,11 +11580,14 @@
       <c r="H290" s="2">
         <v>107187905</v>
       </c>
-      <c r="I290" s="5">
+      <c r="I290" s="1">
         <v>17533</v>
       </c>
-    </row>
-    <row r="291" spans="1:9">
+      <c r="J290" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="291" spans="1:10">
       <c r="A291">
         <v>8234</v>
       </c>
@@ -11125,11 +11612,14 @@
       <c r="H291" s="2">
         <v>107187905</v>
       </c>
-      <c r="I291" s="5">
+      <c r="I291" s="1">
         <v>17533</v>
       </c>
-    </row>
-    <row r="292" spans="1:9">
+      <c r="J291" s="1">
+        <v>17530</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10">
       <c r="A292">
         <v>8255</v>
       </c>
@@ -11154,11 +11644,14 @@
       <c r="H292" s="2">
         <v>107321461</v>
       </c>
-      <c r="I292" s="5">
+      <c r="I292" s="1">
         <v>41360</v>
       </c>
-    </row>
-    <row r="293" spans="1:9">
+      <c r="J292" s="1">
+        <v>41361</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10">
       <c r="A293">
         <v>8272</v>
       </c>
@@ -11183,11 +11676,12 @@
       <c r="H293" s="2">
         <v>105477108</v>
       </c>
-      <c r="I293" s="5">
+      <c r="I293" s="1">
         <v>35352</v>
       </c>
-    </row>
-    <row r="294" spans="1:9">
+      <c r="J293" s="1"/>
+    </row>
+    <row r="294" spans="1:10">
       <c r="A294">
         <v>8291</v>
       </c>
@@ -11212,9 +11706,10 @@
       <c r="H294" s="2">
         <v>106900555</v>
       </c>
-      <c r="I294" s="5">
+      <c r="I294" s="1">
         <v>16811</v>
       </c>
+      <c r="J294" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
revisi error and reference sales report
</commit_message>
<xml_diff>
--- a/postal_error.xlsx
+++ b/postal_error.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="528">
   <si>
     <t>MYRKETAPANG</t>
   </si>
@@ -1603,7 +1603,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19">
     <font>
       <sz val="11"/>
@@ -2377,9 +2377,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J294" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
-  <autoFilter ref="A1:J294">
-    <filterColumn colId="9"/>
-  </autoFilter>
+  <autoFilter ref="A1:J294"/>
   <tableColumns count="10">
     <tableColumn id="1" name="ROW"/>
     <tableColumn id="2" name="COMPANY REFERENCE"/>
@@ -2685,18 +2683,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C270" workbookViewId="0">
-      <selection activeCell="J284" sqref="J284"/>
+    <sheetView tabSelected="1" topLeftCell="C26" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3411,7 +3409,9 @@
       <c r="I22" s="1">
         <v>41334</v>
       </c>
-      <c r="J22" s="1"/>
+      <c r="J22" s="1">
+        <v>41361</v>
+      </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23">
@@ -3441,7 +3441,9 @@
       <c r="I23" s="1">
         <v>11222</v>
       </c>
-      <c r="J23" s="1"/>
+      <c r="J23" s="1" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24">
@@ -3471,7 +3473,9 @@
       <c r="I24" s="1">
         <v>16472</v>
       </c>
-      <c r="J24" s="1"/>
+      <c r="J24" s="1">
+        <v>16433</v>
+      </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25">
@@ -3501,7 +3505,9 @@
       <c r="I25" s="1">
         <v>15811</v>
       </c>
-      <c r="J25" s="1"/>
+      <c r="J25" s="1">
+        <v>15810</v>
+      </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26">
@@ -3563,7 +3569,9 @@
       <c r="I27" s="1">
         <v>15811</v>
       </c>
-      <c r="J27" s="1"/>
+      <c r="J27" s="1">
+        <v>15810</v>
+      </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28">
@@ -3657,7 +3665,9 @@
       <c r="I30" s="1">
         <v>15811</v>
       </c>
-      <c r="J30" s="1"/>
+      <c r="J30" s="1">
+        <v>15810</v>
+      </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31">
@@ -3687,7 +3697,9 @@
       <c r="I31" s="1">
         <v>16952</v>
       </c>
-      <c r="J31" s="1"/>
+      <c r="J31" s="1">
+        <v>16416</v>
+      </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32">
@@ -3781,7 +3793,9 @@
       <c r="I34" s="1">
         <v>42435</v>
       </c>
-      <c r="J34" s="1"/>
+      <c r="J34" s="1">
+        <v>42416</v>
+      </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35">
@@ -3843,7 +3857,9 @@
       <c r="I36" s="1">
         <v>40298</v>
       </c>
-      <c r="J36" s="1"/>
+      <c r="J36" s="1">
+        <v>40112</v>
+      </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37">
@@ -3873,7 +3889,9 @@
       <c r="I37" s="1">
         <v>41326</v>
       </c>
-      <c r="J37" s="1"/>
+      <c r="J37" s="1">
+        <v>41317</v>
+      </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38">
@@ -4025,7 +4043,9 @@
       <c r="I42" s="1">
         <v>41326</v>
       </c>
-      <c r="J42" s="1"/>
+      <c r="J42" s="1">
+        <v>41317</v>
+      </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43">
@@ -4543,7 +4563,9 @@
       <c r="I59" s="1">
         <v>16952</v>
       </c>
-      <c r="J59" s="1"/>
+      <c r="J59" s="1">
+        <v>16416</v>
+      </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60">
@@ -6597,7 +6619,9 @@
       <c r="I126" s="1">
         <v>15811</v>
       </c>
-      <c r="J126" s="1"/>
+      <c r="J126" s="1">
+        <v>15810</v>
+      </c>
     </row>
     <row r="127" spans="1:10">
       <c r="A127">
@@ -10357,7 +10381,9 @@
       <c r="I250" s="1">
         <v>41326</v>
       </c>
-      <c r="J250" s="1"/>
+      <c r="J250" s="1">
+        <v>41317</v>
+      </c>
     </row>
     <row r="251" spans="1:10">
       <c r="A251">

</xml_diff>

<commit_message>
nyicil refactory postal error
</commit_message>
<xml_diff>
--- a/postal_error.xlsx
+++ b/postal_error.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="528">
   <si>
     <t>MYRKETAPANG</t>
   </si>
@@ -1603,7 +1603,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="19">
     <font>
       <sz val="11"/>
@@ -2683,18 +2683,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C26" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="C91" workbookViewId="0">
+      <selection activeCell="I95" sqref="I95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2865,8 +2865,8 @@
       <c r="I5" s="1">
         <v>16270</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>527</v>
+      <c r="J5" s="1">
+        <v>16430</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3953,7 +3953,9 @@
       <c r="I39" s="1">
         <v>40199</v>
       </c>
-      <c r="J39" s="1"/>
+      <c r="J39" s="1">
+        <v>41271</v>
+      </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40">
@@ -3983,7 +3985,9 @@
       <c r="I40" s="1">
         <v>40296</v>
       </c>
-      <c r="J40" s="1"/>
+      <c r="J40" s="1">
+        <v>40294</v>
+      </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41">
@@ -4013,7 +4017,9 @@
       <c r="I41" s="1">
         <v>41180</v>
       </c>
-      <c r="J41" s="1"/>
+      <c r="J41" s="1">
+        <v>41181</v>
+      </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42">
@@ -4107,7 +4113,9 @@
       <c r="I44" s="1">
         <v>17534</v>
       </c>
-      <c r="J44" s="1"/>
+      <c r="J44" s="1">
+        <v>17530</v>
+      </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45">
@@ -4137,7 +4145,9 @@
       <c r="I45" s="1">
         <v>15721</v>
       </c>
-      <c r="J45" s="1"/>
+      <c r="J45" s="1">
+        <v>15720</v>
+      </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46">
@@ -4199,7 +4209,9 @@
       <c r="I47" s="1">
         <v>17534</v>
       </c>
-      <c r="J47" s="1"/>
+      <c r="J47" s="1">
+        <v>17530</v>
+      </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48">
@@ -4229,7 +4241,9 @@
       <c r="I48" s="1">
         <v>45159</v>
       </c>
-      <c r="J48" s="1"/>
+      <c r="J48" s="1">
+        <v>45154</v>
+      </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49">
@@ -4259,7 +4273,9 @@
       <c r="I49" s="1">
         <v>16672</v>
       </c>
-      <c r="J49" s="1"/>
+      <c r="J49" s="1">
+        <v>16670</v>
+      </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50">
@@ -4289,7 +4305,9 @@
       <c r="I50" s="1">
         <v>17534</v>
       </c>
-      <c r="J50" s="1"/>
+      <c r="J50" s="1">
+        <v>17530</v>
+      </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51">
@@ -4319,7 +4337,9 @@
       <c r="I51" s="1">
         <v>15853</v>
       </c>
-      <c r="J51" s="1"/>
+      <c r="J51" s="1">
+        <v>15820</v>
+      </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52">
@@ -4381,7 +4401,9 @@
       <c r="I53" s="1">
         <v>17534</v>
       </c>
-      <c r="J53" s="1"/>
+      <c r="J53" s="1">
+        <v>17530</v>
+      </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54">
@@ -4411,7 +4433,9 @@
       <c r="I54" s="1">
         <v>16270</v>
       </c>
-      <c r="J54" s="1"/>
+      <c r="J54" s="1">
+        <v>16340</v>
+      </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55">
@@ -4473,7 +4497,9 @@
       <c r="I56" s="1">
         <v>16378</v>
       </c>
-      <c r="J56" s="1"/>
+      <c r="J56" s="1">
+        <v>16370</v>
+      </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57">
@@ -4503,7 +4529,9 @@
       <c r="I57" s="1">
         <v>40754</v>
       </c>
-      <c r="J57" s="1"/>
+      <c r="J57" s="1">
+        <v>40554</v>
+      </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58">
@@ -4533,7 +4561,9 @@
       <c r="I58" s="1">
         <v>15711</v>
       </c>
-      <c r="J58" s="1"/>
+      <c r="J58" s="1">
+        <v>15710</v>
+      </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59">
@@ -4595,7 +4625,9 @@
       <c r="I60" s="1">
         <v>16285</v>
       </c>
-      <c r="J60" s="1"/>
+      <c r="J60" s="1">
+        <v>16640</v>
+      </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61">
@@ -4689,7 +4721,9 @@
       <c r="I63" s="1">
         <v>16811</v>
       </c>
-      <c r="J63" s="1"/>
+      <c r="J63" s="1">
+        <v>16810</v>
+      </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64">
@@ -4719,7 +4753,9 @@
       <c r="I64" s="1">
         <v>43286</v>
       </c>
-      <c r="J64" s="1"/>
+      <c r="J64" s="1">
+        <v>43284</v>
+      </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65">
@@ -4749,7 +4785,9 @@
       <c r="I65" s="1">
         <v>40355</v>
       </c>
-      <c r="J65" s="1"/>
+      <c r="J65" s="1">
+        <v>78821</v>
+      </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66">
@@ -4779,7 +4817,9 @@
       <c r="I66" s="1">
         <v>16387</v>
       </c>
-      <c r="J66" s="1"/>
+      <c r="J66" s="1">
+        <v>16120</v>
+      </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67">
@@ -4841,7 +4881,9 @@
       <c r="I68" s="1">
         <v>16872</v>
       </c>
-      <c r="J68" s="1"/>
+      <c r="J68" s="1">
+        <v>16710</v>
+      </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69">
@@ -4871,7 +4913,9 @@
       <c r="I69" s="1">
         <v>16772</v>
       </c>
-      <c r="J69" s="1"/>
+      <c r="J69" s="1">
+        <v>16770</v>
+      </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70">
@@ -4933,7 +4977,9 @@
       <c r="I71" s="1">
         <v>40762</v>
       </c>
-      <c r="J71" s="1"/>
+      <c r="J71" s="1">
+        <v>40562</v>
+      </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72">
@@ -4963,7 +5009,9 @@
       <c r="I72" s="1">
         <v>16831</v>
       </c>
-      <c r="J72" s="1"/>
+      <c r="J72" s="1">
+        <v>16830</v>
+      </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73">
@@ -5025,7 +5073,9 @@
       <c r="I74" s="1">
         <v>40354</v>
       </c>
-      <c r="J74" s="1"/>
+      <c r="J74" s="1">
+        <v>40288</v>
+      </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75">
@@ -5055,7 +5105,9 @@
       <c r="I75" s="1">
         <v>16785</v>
       </c>
-      <c r="J75" s="1"/>
+      <c r="J75" s="1">
+        <v>16740</v>
+      </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76">
@@ -5117,7 +5169,9 @@
       <c r="I77" s="1">
         <v>15721</v>
       </c>
-      <c r="J77" s="1"/>
+      <c r="J77" s="1">
+        <v>15720</v>
+      </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78">
@@ -5147,7 +5201,9 @@
       <c r="I78" s="1">
         <v>16759</v>
       </c>
-      <c r="J78" s="1"/>
+      <c r="J78" s="1">
+        <v>16750</v>
+      </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79">
@@ -5177,7 +5233,9 @@
       <c r="I79" s="1">
         <v>45160</v>
       </c>
-      <c r="J79" s="1"/>
+      <c r="J79" s="1">
+        <v>45161</v>
+      </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80">
@@ -5239,7 +5297,9 @@
       <c r="I81" s="1">
         <v>16927</v>
       </c>
-      <c r="J81" s="1"/>
+      <c r="J81" s="1">
+        <v>16922</v>
+      </c>
     </row>
     <row r="82" spans="1:10">
       <c r="A82">
@@ -5269,7 +5329,9 @@
       <c r="I82" s="1">
         <v>40193</v>
       </c>
-      <c r="J82" s="1"/>
+      <c r="J82" s="1">
+        <v>40195</v>
+      </c>
     </row>
     <row r="83" spans="1:10">
       <c r="A83">
@@ -5299,7 +5361,9 @@
       <c r="I83" s="1">
         <v>17163</v>
       </c>
-      <c r="J83" s="1"/>
+      <c r="J83" s="1">
+        <v>17132</v>
+      </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84">
@@ -5329,7 +5393,9 @@
       <c r="I84" s="1">
         <v>16951</v>
       </c>
-      <c r="J84" s="1"/>
+      <c r="J84" s="1">
+        <v>16451</v>
+      </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85">
@@ -5391,7 +5457,9 @@
       <c r="I86" s="1">
         <v>40974</v>
       </c>
-      <c r="J86" s="1"/>
+      <c r="J86" s="1">
+        <v>40973</v>
+      </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87">
@@ -5453,7 +5521,9 @@
       <c r="I88" s="1">
         <v>16811</v>
       </c>
-      <c r="J88" s="1"/>
+      <c r="J88" s="1">
+        <v>16810</v>
+      </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89">
@@ -5483,7 +5553,9 @@
       <c r="I89" s="1">
         <v>16811</v>
       </c>
-      <c r="J89" s="1"/>
+      <c r="J89" s="1">
+        <v>16810</v>
+      </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90">
@@ -5513,7 +5585,9 @@
       <c r="I90" s="1">
         <v>16811</v>
       </c>
-      <c r="J90" s="1"/>
+      <c r="J90" s="1">
+        <v>16810</v>
+      </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91">
@@ -5543,7 +5617,9 @@
       <c r="I91" s="1">
         <v>15711</v>
       </c>
-      <c r="J91" s="1"/>
+      <c r="J91" s="1">
+        <v>15710</v>
+      </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92">
@@ -5573,7 +5649,9 @@
       <c r="I92" s="1">
         <v>16661</v>
       </c>
-      <c r="J92" s="1"/>
+      <c r="J92" s="1">
+        <v>16660</v>
+      </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93">
@@ -5603,7 +5681,9 @@
       <c r="I93" s="1">
         <v>40560</v>
       </c>
-      <c r="J93" s="1"/>
+      <c r="J93" s="1">
+        <v>40561</v>
+      </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94">
@@ -5633,7 +5713,9 @@
       <c r="I94" s="1">
         <v>44179</v>
       </c>
-      <c r="J94" s="1"/>
+      <c r="J94" s="1">
+        <v>44184</v>
+      </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95">
@@ -5663,7 +5745,9 @@
       <c r="I95" s="1">
         <v>15561</v>
       </c>
-      <c r="J95" s="1"/>
+      <c r="J95" s="1">
+        <v>15560</v>
+      </c>
     </row>
     <row r="96" spans="1:10">
       <c r="A96">
@@ -5693,7 +5777,9 @@
       <c r="I96" s="1">
         <v>17631</v>
       </c>
-      <c r="J96" s="1"/>
+      <c r="J96" s="1">
+        <v>17630</v>
+      </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97">
@@ -5723,7 +5809,9 @@
       <c r="I97" s="1">
         <v>46191</v>
       </c>
-      <c r="J97" s="1"/>
+      <c r="J97" s="1">
+        <v>46196</v>
+      </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98">
@@ -5785,7 +5873,9 @@
       <c r="I99" s="1">
         <v>40296</v>
       </c>
-      <c r="J99" s="1"/>
+      <c r="J99" s="1">
+        <v>40294</v>
+      </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100">
@@ -5847,7 +5937,9 @@
       <c r="I101" s="1">
         <v>41375</v>
       </c>
-      <c r="J101" s="1"/>
+      <c r="J101" s="1">
+        <v>41374</v>
+      </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102">
@@ -5877,7 +5969,9 @@
       <c r="I102" s="1">
         <v>45159</v>
       </c>
-      <c r="J102" s="1"/>
+      <c r="J102" s="1">
+        <v>45154</v>
+      </c>
     </row>
     <row r="103" spans="1:10">
       <c r="A103">
@@ -5907,7 +6001,9 @@
       <c r="I103" s="1">
         <v>15611</v>
       </c>
-      <c r="J103" s="1"/>
+      <c r="J103" s="1">
+        <v>15610</v>
+      </c>
     </row>
     <row r="104" spans="1:10">
       <c r="A104">
@@ -5969,7 +6065,9 @@
       <c r="I105" s="1">
         <v>41180</v>
       </c>
-      <c r="J105" s="1"/>
+      <c r="J105" s="1">
+        <v>41181</v>
+      </c>
     </row>
     <row r="106" spans="1:10">
       <c r="A106">
@@ -6031,7 +6129,9 @@
       <c r="I107" s="1">
         <v>45360</v>
       </c>
-      <c r="J107" s="1"/>
+      <c r="J107" s="1">
+        <v>45363</v>
+      </c>
     </row>
     <row r="108" spans="1:10">
       <c r="A108">
@@ -6061,7 +6161,9 @@
       <c r="I108" s="1">
         <v>40567</v>
       </c>
-      <c r="J108" s="1"/>
+      <c r="J108" s="1">
+        <v>40562</v>
+      </c>
     </row>
     <row r="109" spans="1:10">
       <c r="A109">
@@ -6091,7 +6193,9 @@
       <c r="I109" s="1">
         <v>44150</v>
       </c>
-      <c r="J109" s="1"/>
+      <c r="J109" s="1">
+        <v>44151</v>
+      </c>
     </row>
     <row r="110" spans="1:10">
       <c r="A110">
@@ -6153,7 +6257,9 @@
       <c r="I111" s="1">
         <v>60168</v>
       </c>
-      <c r="J111" s="1"/>
+      <c r="J111" s="1">
+        <v>60183</v>
+      </c>
     </row>
     <row r="112" spans="1:10">
       <c r="A112">
@@ -6183,7 +6289,9 @@
       <c r="I112" s="1">
         <v>41376</v>
       </c>
-      <c r="J112" s="1"/>
+      <c r="J112" s="1">
+        <v>41374</v>
+      </c>
     </row>
     <row r="113" spans="1:10">
       <c r="A113">
@@ -6277,7 +6385,9 @@
       <c r="I115" s="1">
         <v>41364</v>
       </c>
-      <c r="J115" s="1"/>
+      <c r="J115" s="1">
+        <v>41362</v>
+      </c>
     </row>
     <row r="116" spans="1:10">
       <c r="A116">
@@ -6307,7 +6417,9 @@
       <c r="I116" s="1">
         <v>17535</v>
       </c>
-      <c r="J116" s="1"/>
+      <c r="J116" s="1">
+        <v>17530</v>
+      </c>
     </row>
     <row r="117" spans="1:10">
       <c r="A117">
@@ -6337,7 +6449,9 @@
       <c r="I117" s="1">
         <v>15532</v>
       </c>
-      <c r="J117" s="1"/>
+      <c r="J117" s="1">
+        <v>15530</v>
+      </c>
     </row>
     <row r="118" spans="1:10">
       <c r="A118">
@@ -6463,7 +6577,9 @@
       <c r="I121" s="1">
         <v>17631</v>
       </c>
-      <c r="J121" s="1"/>
+      <c r="J121" s="1">
+        <v>17630</v>
+      </c>
     </row>
     <row r="122" spans="1:10">
       <c r="A122">
@@ -6525,7 +6641,9 @@
       <c r="I123" s="1">
         <v>17621</v>
       </c>
-      <c r="J123" s="1"/>
+      <c r="J123" s="1">
+        <v>17620</v>
+      </c>
     </row>
     <row r="124" spans="1:10">
       <c r="A124">
@@ -6651,7 +6769,9 @@
       <c r="I127" s="1">
         <v>40296</v>
       </c>
-      <c r="J127" s="1"/>
+      <c r="J127" s="1">
+        <v>40294</v>
+      </c>
     </row>
     <row r="128" spans="1:10">
       <c r="A128">
@@ -6681,7 +6801,9 @@
       <c r="I128" s="1">
         <v>44150</v>
       </c>
-      <c r="J128" s="1"/>
+      <c r="J128" s="1">
+        <v>44151</v>
+      </c>
     </row>
     <row r="129" spans="1:10">
       <c r="A129">
@@ -6711,7 +6833,9 @@
       <c r="I129" s="1">
         <v>15721</v>
       </c>
-      <c r="J129" s="1"/>
+      <c r="J129" s="1">
+        <v>15720</v>
+      </c>
     </row>
     <row r="130" spans="1:10">
       <c r="A130">
@@ -6741,7 +6865,9 @@
       <c r="I130" s="1">
         <v>51157</v>
       </c>
-      <c r="J130" s="1"/>
+      <c r="J130" s="1">
+        <v>51137</v>
+      </c>
     </row>
     <row r="131" spans="1:10">
       <c r="A131">
@@ -6771,7 +6897,9 @@
       <c r="I131" s="1">
         <v>12610</v>
       </c>
-      <c r="J131" s="1"/>
+      <c r="J131" s="1">
+        <v>12620</v>
+      </c>
     </row>
     <row r="132" spans="1:10">
       <c r="A132">
@@ -6801,7 +6929,9 @@
       <c r="I132" s="1">
         <v>61728</v>
       </c>
-      <c r="J132" s="1"/>
+      <c r="J132" s="1">
+        <v>61372</v>
+      </c>
     </row>
     <row r="133" spans="1:10">
       <c r="A133">
@@ -6831,7 +6961,9 @@
       <c r="I133" s="1">
         <v>57771</v>
       </c>
-      <c r="J133" s="1"/>
+      <c r="J133" s="1">
+        <v>57731</v>
+      </c>
     </row>
     <row r="134" spans="1:10">
       <c r="A134">
@@ -6861,7 +6993,9 @@
       <c r="I134" s="1">
         <v>67724</v>
       </c>
-      <c r="J134" s="1"/>
+      <c r="J134" s="1">
+        <v>67225</v>
+      </c>
     </row>
     <row r="135" spans="1:10">
       <c r="A135">
@@ -6891,7 +7025,9 @@
       <c r="I135" s="1">
         <v>61301</v>
       </c>
-      <c r="J135" s="1"/>
+      <c r="J135" s="1">
+        <v>61265</v>
+      </c>
     </row>
     <row r="136" spans="1:10">
       <c r="A136">
@@ -6921,7 +7057,9 @@
       <c r="I136" s="1">
         <v>61301</v>
       </c>
-      <c r="J136" s="1"/>
+      <c r="J136" s="1">
+        <v>61265</v>
+      </c>
     </row>
     <row r="137" spans="1:10">
       <c r="A137">
@@ -6951,7 +7089,9 @@
       <c r="I137" s="1">
         <v>64412</v>
       </c>
-      <c r="J137" s="1"/>
+      <c r="J137" s="1">
+        <v>64411</v>
+      </c>
     </row>
     <row r="138" spans="1:10">
       <c r="A138">
@@ -6981,7 +7121,9 @@
       <c r="I138" s="1">
         <v>57771</v>
       </c>
-      <c r="J138" s="1"/>
+      <c r="J138" s="1">
+        <v>57731</v>
+      </c>
     </row>
     <row r="139" spans="1:10">
       <c r="A139">
@@ -7011,7 +7153,9 @@
       <c r="I139" s="1">
         <v>45126</v>
       </c>
-      <c r="J139" s="1"/>
+      <c r="J139" s="1">
+        <v>46125</v>
+      </c>
     </row>
     <row r="140" spans="1:10">
       <c r="A140">
@@ -7041,7 +7185,9 @@
       <c r="I140" s="1">
         <v>61532</v>
       </c>
-      <c r="J140" s="1"/>
+      <c r="J140" s="1">
+        <v>61352</v>
+      </c>
     </row>
     <row r="141" spans="1:10">
       <c r="A141">
@@ -7071,7 +7217,9 @@
       <c r="I141" s="1">
         <v>57771</v>
       </c>
-      <c r="J141" s="1"/>
+      <c r="J141" s="1">
+        <v>57731</v>
+      </c>
     </row>
     <row r="142" spans="1:10">
       <c r="A142">
@@ -7101,7 +7249,9 @@
       <c r="I142" s="1">
         <v>57771</v>
       </c>
-      <c r="J142" s="1"/>
+      <c r="J142" s="1">
+        <v>57731</v>
+      </c>
     </row>
     <row r="143" spans="1:10">
       <c r="A143">
@@ -7163,7 +7313,9 @@
       <c r="I144" s="1">
         <v>64412</v>
       </c>
-      <c r="J144" s="1"/>
+      <c r="J144" s="1">
+        <v>64411</v>
+      </c>
     </row>
     <row r="145" spans="1:10">
       <c r="A145">
@@ -7193,7 +7345,9 @@
       <c r="I145" s="1">
         <v>64412</v>
       </c>
-      <c r="J145" s="1"/>
+      <c r="J145" s="1">
+        <v>64411</v>
+      </c>
     </row>
     <row r="146" spans="1:10">
       <c r="A146">
@@ -7223,7 +7377,9 @@
       <c r="I146" s="1">
         <v>41288</v>
       </c>
-      <c r="J146" s="1"/>
+      <c r="J146" s="1">
+        <v>41282</v>
+      </c>
     </row>
     <row r="147" spans="1:10">
       <c r="A147">
@@ -7253,7 +7409,9 @@
       <c r="I147" s="1">
         <v>16811</v>
       </c>
-      <c r="J147" s="1"/>
+      <c r="J147" s="1">
+        <v>16810</v>
+      </c>
     </row>
     <row r="148" spans="1:10">
       <c r="A148">
@@ -7283,7 +7441,9 @@
       <c r="I148" s="1">
         <v>61326</v>
       </c>
-      <c r="J148" s="1"/>
+      <c r="J148" s="1">
+        <v>61328</v>
+      </c>
     </row>
     <row r="149" spans="1:10">
       <c r="A149">
@@ -7313,7 +7473,9 @@
       <c r="I149" s="1">
         <v>57771</v>
       </c>
-      <c r="J149" s="1"/>
+      <c r="J149" s="1">
+        <v>57731</v>
+      </c>
     </row>
     <row r="150" spans="1:10">
       <c r="A150">
@@ -7373,7 +7535,9 @@
       <c r="I151" s="1">
         <v>16811</v>
       </c>
-      <c r="J151" s="1"/>
+      <c r="J151" s="1">
+        <v>16810</v>
+      </c>
     </row>
     <row r="152" spans="1:10">
       <c r="A152">
@@ -7527,7 +7691,9 @@
       <c r="I156" s="1">
         <v>57771</v>
       </c>
-      <c r="J156" s="1"/>
+      <c r="J156" s="1">
+        <v>57731</v>
+      </c>
     </row>
     <row r="157" spans="1:10">
       <c r="A157">
@@ -7557,7 +7723,9 @@
       <c r="I157" s="1">
         <v>57771</v>
       </c>
-      <c r="J157" s="1"/>
+      <c r="J157" s="1">
+        <v>57731</v>
+      </c>
     </row>
     <row r="158" spans="1:10">
       <c r="A158">
@@ -7835,7 +8003,9 @@
       <c r="I166" s="1">
         <v>16811</v>
       </c>
-      <c r="J166" s="1"/>
+      <c r="J166" s="1">
+        <v>16810</v>
+      </c>
     </row>
     <row r="167" spans="1:10">
       <c r="A167">
@@ -7955,7 +8125,9 @@
       <c r="I170" s="1">
         <v>15561</v>
       </c>
-      <c r="J170" s="1"/>
+      <c r="J170" s="1">
+        <v>15560</v>
+      </c>
     </row>
     <row r="171" spans="1:10">
       <c r="A171">
@@ -8105,7 +8277,9 @@
       <c r="I175" s="1">
         <v>15721</v>
       </c>
-      <c r="J175" s="1"/>
+      <c r="J175" s="1">
+        <v>15720</v>
+      </c>
     </row>
     <row r="176" spans="1:10">
       <c r="A176">
@@ -8889,7 +9063,9 @@
       <c r="I201" s="1">
         <v>15561</v>
       </c>
-      <c r="J201" s="1"/>
+      <c r="J201" s="1">
+        <v>15560</v>
+      </c>
     </row>
     <row r="202" spans="1:10">
       <c r="A202">
@@ -9345,7 +9521,9 @@
       <c r="I216" s="1">
         <v>41376</v>
       </c>
-      <c r="J216" s="1"/>
+      <c r="J216" s="1">
+        <v>41374</v>
+      </c>
     </row>
     <row r="217" spans="1:10">
       <c r="A217">
@@ -9495,7 +9673,9 @@
       <c r="I221" s="1">
         <v>40296</v>
       </c>
-      <c r="J221" s="1"/>
+      <c r="J221" s="1">
+        <v>40294</v>
+      </c>
     </row>
     <row r="222" spans="1:10">
       <c r="A222">
@@ -9525,7 +9705,9 @@
       <c r="I222" s="1">
         <v>40296</v>
       </c>
-      <c r="J222" s="1"/>
+      <c r="J222" s="1">
+        <v>40294</v>
+      </c>
     </row>
     <row r="223" spans="1:10">
       <c r="A223">
@@ -9615,7 +9797,9 @@
       <c r="I225" s="1">
         <v>15561</v>
       </c>
-      <c r="J225" s="1"/>
+      <c r="J225" s="1">
+        <v>15560</v>
+      </c>
     </row>
     <row r="226" spans="1:10">
       <c r="A226">
@@ -9893,7 +10077,9 @@
       <c r="I234" s="1">
         <v>41376</v>
       </c>
-      <c r="J234" s="1"/>
+      <c r="J234" s="1">
+        <v>41374</v>
+      </c>
     </row>
     <row r="235" spans="1:10">
       <c r="A235">
@@ -9923,7 +10109,9 @@
       <c r="I235" s="1">
         <v>40296</v>
       </c>
-      <c r="J235" s="1"/>
+      <c r="J235" s="1">
+        <v>40294</v>
+      </c>
     </row>
     <row r="236" spans="1:10">
       <c r="A236">
@@ -9983,7 +10171,9 @@
       <c r="I237" s="1">
         <v>57771</v>
       </c>
-      <c r="J237" s="1"/>
+      <c r="J237" s="1">
+        <v>57731</v>
+      </c>
     </row>
     <row r="238" spans="1:10">
       <c r="A238">
@@ -10197,7 +10387,9 @@
       <c r="I244" s="1">
         <v>41376</v>
       </c>
-      <c r="J244" s="1"/>
+      <c r="J244" s="1">
+        <v>41374</v>
+      </c>
     </row>
     <row r="245" spans="1:10">
       <c r="A245">
@@ -10505,7 +10697,9 @@
       <c r="I254" s="1">
         <v>16811</v>
       </c>
-      <c r="J254" s="1"/>
+      <c r="J254" s="1">
+        <v>16810</v>
+      </c>
     </row>
     <row r="255" spans="1:10">
       <c r="A255">
@@ -10751,7 +10945,9 @@
       <c r="I262" s="1">
         <v>45159</v>
       </c>
-      <c r="J262" s="1"/>
+      <c r="J262" s="1">
+        <v>45154</v>
+      </c>
     </row>
     <row r="263" spans="1:10">
       <c r="A263">
@@ -10877,7 +11073,9 @@
       <c r="I266" s="1">
         <v>16811</v>
       </c>
-      <c r="J266" s="1"/>
+      <c r="J266" s="1">
+        <v>16810</v>
+      </c>
     </row>
     <row r="267" spans="1:10">
       <c r="A267">
@@ -10937,7 +11135,9 @@
       <c r="I268" s="1">
         <v>16811</v>
       </c>
-      <c r="J268" s="1"/>
+      <c r="J268" s="1">
+        <v>16810</v>
+      </c>
     </row>
     <row r="269" spans="1:10">
       <c r="A269">
@@ -11029,7 +11229,9 @@
       <c r="I271" s="1">
         <v>40296</v>
       </c>
-      <c r="J271" s="1"/>
+      <c r="J271" s="1">
+        <v>40294</v>
+      </c>
     </row>
     <row r="272" spans="1:10">
       <c r="A272">
@@ -11091,7 +11293,9 @@
       <c r="I273" s="1">
         <v>45159</v>
       </c>
-      <c r="J273" s="1"/>
+      <c r="J273" s="1">
+        <v>45154</v>
+      </c>
     </row>
     <row r="274" spans="1:10">
       <c r="A274">
@@ -11211,7 +11415,9 @@
       <c r="I277" s="1">
         <v>16811</v>
       </c>
-      <c r="J277" s="1"/>
+      <c r="J277" s="1">
+        <v>16810</v>
+      </c>
     </row>
     <row r="278" spans="1:10">
       <c r="A278">
@@ -11271,7 +11477,9 @@
       <c r="I279" s="1">
         <v>41376</v>
       </c>
-      <c r="J279" s="1"/>
+      <c r="J279" s="1">
+        <v>41374</v>
+      </c>
     </row>
     <row r="280" spans="1:10">
       <c r="A280">
@@ -11331,7 +11539,9 @@
       <c r="I281" s="1">
         <v>51157</v>
       </c>
-      <c r="J281" s="1"/>
+      <c r="J281" s="1">
+        <v>51137</v>
+      </c>
     </row>
     <row r="282" spans="1:10">
       <c r="A282">
@@ -11361,7 +11571,9 @@
       <c r="I282" s="1">
         <v>41180</v>
       </c>
-      <c r="J282" s="1"/>
+      <c r="J282" s="1">
+        <v>41181</v>
+      </c>
     </row>
     <row r="283" spans="1:10">
       <c r="A283">
@@ -11455,7 +11667,9 @@
       <c r="I285" s="1">
         <v>16811</v>
       </c>
-      <c r="J285" s="1"/>
+      <c r="J285" s="1">
+        <v>16810</v>
+      </c>
     </row>
     <row r="286" spans="1:10">
       <c r="A286">
@@ -11579,7 +11793,9 @@
       <c r="I289" s="1">
         <v>15611</v>
       </c>
-      <c r="J289" s="1"/>
+      <c r="J289" s="1">
+        <v>15610</v>
+      </c>
     </row>
     <row r="290" spans="1:10">
       <c r="A290">
@@ -11735,7 +11951,9 @@
       <c r="I294" s="1">
         <v>16811</v>
       </c>
-      <c r="J294" s="1"/>
+      <c r="J294" s="1">
+        <v>16810</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
POSTAL FINAL ERROR FIX
</commit_message>
<xml_diff>
--- a/postal_error.xlsx
+++ b/postal_error.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="528">
   <si>
     <t>MYRKETAPANG</t>
   </si>
@@ -1747,7 +1747,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1925,6 +1925,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2125,13 +2131,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2683,7 +2691,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2693,8 +2701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C91" workbookViewId="0">
-      <selection activeCell="I95" sqref="I95"/>
+    <sheetView tabSelected="1" topLeftCell="C286" workbookViewId="0">
+      <selection activeCell="E294" sqref="E294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3253,35 +3261,35 @@
         <v>43261</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18">
+    <row r="18" spans="1:10" s="6" customFormat="1">
+      <c r="A18" s="6">
         <v>744</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="1">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1">
+      <c r="G18" s="7">
+        <v>0</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0</v>
+      </c>
+      <c r="I18" s="7">
         <v>40352</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J18" s="7" t="s">
         <v>527</v>
       </c>
     </row>
@@ -3413,35 +3421,35 @@
         <v>41361</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23">
+    <row r="23" spans="1:10" s="6" customFormat="1">
+      <c r="A23" s="6">
         <v>873</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G23" s="1">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0</v>
-      </c>
-      <c r="I23" s="1">
+      <c r="G23" s="7">
+        <v>0</v>
+      </c>
+      <c r="H23" s="7">
+        <v>0</v>
+      </c>
+      <c r="I23" s="7">
         <v>11222</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="J23" s="7" t="s">
         <v>527</v>
       </c>
     </row>
@@ -7477,35 +7485,37 @@
         <v>57731</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
-      <c r="A150">
+    <row r="150" spans="1:10" s="6" customFormat="1">
+      <c r="A150" s="6">
         <v>4388</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B150" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="C150" s="1" t="s">
+      <c r="C150" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="D150" s="1" t="s">
+      <c r="D150" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="E150" s="1" t="s">
+      <c r="E150" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="F150" s="1" t="s">
+      <c r="F150" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="G150" s="1">
-        <v>0</v>
-      </c>
-      <c r="H150" s="1">
-        <v>0</v>
-      </c>
-      <c r="I150" s="1">
+      <c r="G150" s="7">
+        <v>0</v>
+      </c>
+      <c r="H150" s="7">
+        <v>0</v>
+      </c>
+      <c r="I150" s="7">
         <v>55501</v>
       </c>
-      <c r="J150" s="1"/>
+      <c r="J150" s="7" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="151" spans="1:10">
       <c r="A151">
@@ -7567,7 +7577,9 @@
       <c r="I152" s="1">
         <v>61251</v>
       </c>
-      <c r="J152" s="1"/>
+      <c r="J152" s="1">
+        <v>61252</v>
+      </c>
     </row>
     <row r="153" spans="1:10">
       <c r="A153">
@@ -7597,7 +7609,9 @@
       <c r="I153" s="1">
         <v>41287</v>
       </c>
-      <c r="J153" s="1"/>
+      <c r="J153" s="1">
+        <v>41283</v>
+      </c>
     </row>
     <row r="154" spans="1:10">
       <c r="A154">
@@ -7787,7 +7801,9 @@
       <c r="I159" s="1">
         <v>17750</v>
       </c>
-      <c r="J159" s="1"/>
+      <c r="J159" s="1">
+        <v>17530</v>
+      </c>
     </row>
     <row r="160" spans="1:10">
       <c r="A160">
@@ -7849,7 +7865,9 @@
       <c r="I161" s="1">
         <v>12345</v>
       </c>
-      <c r="J161" s="1"/>
+      <c r="J161" s="1">
+        <v>17143</v>
+      </c>
     </row>
     <row r="162" spans="1:10">
       <c r="A162">
@@ -7911,7 +7929,9 @@
       <c r="I163" s="1">
         <v>17352</v>
       </c>
-      <c r="J163" s="1"/>
+      <c r="J163" s="1">
+        <v>17350</v>
+      </c>
     </row>
     <row r="164" spans="1:10">
       <c r="A164">
@@ -7941,7 +7961,9 @@
       <c r="I164" s="1">
         <v>17772</v>
       </c>
-      <c r="J164" s="1"/>
+      <c r="J164" s="1">
+        <v>16810</v>
+      </c>
     </row>
     <row r="165" spans="1:10">
       <c r="A165">
@@ -8035,7 +8057,9 @@
       <c r="I167" s="1">
         <v>61464</v>
       </c>
-      <c r="J167" s="1"/>
+      <c r="J167" s="1">
+        <v>61463</v>
+      </c>
     </row>
     <row r="168" spans="1:10">
       <c r="A168">
@@ -8065,7 +8089,9 @@
       <c r="I168" s="1">
         <v>40277</v>
       </c>
-      <c r="J168" s="1"/>
+      <c r="J168" s="1">
+        <v>40227</v>
+      </c>
     </row>
     <row r="169" spans="1:10">
       <c r="A169">
@@ -8095,7 +8121,9 @@
       <c r="I169" s="1">
         <v>40277</v>
       </c>
-      <c r="J169" s="1"/>
+      <c r="J169" s="1">
+        <v>40227</v>
+      </c>
     </row>
     <row r="170" spans="1:10">
       <c r="A170">
@@ -8157,7 +8185,9 @@
       <c r="I171" s="1">
         <v>24252</v>
       </c>
-      <c r="J171" s="1"/>
+      <c r="J171" s="1">
+        <v>24251</v>
+      </c>
     </row>
     <row r="172" spans="1:10">
       <c r="A172">
@@ -8187,7 +8217,9 @@
       <c r="I172" s="1">
         <v>27685</v>
       </c>
-      <c r="J172" s="1"/>
+      <c r="J172" s="1">
+        <v>27684</v>
+      </c>
     </row>
     <row r="173" spans="1:10">
       <c r="A173">
@@ -8217,7 +8249,9 @@
       <c r="I173" s="1">
         <v>28783</v>
       </c>
-      <c r="J173" s="1"/>
+      <c r="J173" s="1">
+        <v>28784</v>
+      </c>
     </row>
     <row r="174" spans="1:10">
       <c r="A174">
@@ -8247,7 +8281,9 @@
       <c r="I174" s="1">
         <v>28553</v>
       </c>
-      <c r="J174" s="1"/>
+      <c r="J174" s="1">
+        <v>28554</v>
+      </c>
     </row>
     <row r="175" spans="1:10">
       <c r="A175">
@@ -8309,7 +8345,9 @@
       <c r="I176" s="1">
         <v>41386</v>
       </c>
-      <c r="J176" s="1"/>
+      <c r="J176" s="1">
+        <v>41384</v>
+      </c>
     </row>
     <row r="177" spans="1:10">
       <c r="A177">
@@ -8339,7 +8377,9 @@
       <c r="I177" s="1">
         <v>22731</v>
       </c>
-      <c r="J177" s="1"/>
+      <c r="J177" s="1">
+        <v>22733</v>
+      </c>
     </row>
     <row r="178" spans="1:10">
       <c r="A178">
@@ -8369,7 +8409,9 @@
       <c r="I178" s="1">
         <v>17352</v>
       </c>
-      <c r="J178" s="1"/>
+      <c r="J178" s="1">
+        <v>17350</v>
+      </c>
     </row>
     <row r="179" spans="1:10">
       <c r="A179">
@@ -8431,7 +8473,9 @@
       <c r="I180" s="1">
         <v>80363</v>
       </c>
-      <c r="J180" s="1"/>
+      <c r="J180" s="1">
+        <v>80361</v>
+      </c>
     </row>
     <row r="181" spans="1:10">
       <c r="A181">
@@ -8461,7 +8505,9 @@
       <c r="I181" s="1">
         <v>28783</v>
       </c>
-      <c r="J181" s="1"/>
+      <c r="J181" s="1">
+        <v>28784</v>
+      </c>
     </row>
     <row r="182" spans="1:10">
       <c r="A182">
@@ -8491,7 +8537,9 @@
       <c r="I182" s="1">
         <v>20272</v>
       </c>
-      <c r="J182" s="1"/>
+      <c r="J182" s="1">
+        <v>20372</v>
+      </c>
     </row>
     <row r="183" spans="1:10">
       <c r="A183">
@@ -8521,7 +8569,9 @@
       <c r="I183" s="1">
         <v>28783</v>
       </c>
-      <c r="J183" s="1"/>
+      <c r="J183" s="1">
+        <v>28784</v>
+      </c>
     </row>
     <row r="184" spans="1:10">
       <c r="A184">
@@ -8551,7 +8601,9 @@
       <c r="I184" s="1">
         <v>20272</v>
       </c>
-      <c r="J184" s="1"/>
+      <c r="J184" s="1">
+        <v>20372</v>
+      </c>
     </row>
     <row r="185" spans="1:10">
       <c r="A185">
@@ -8581,7 +8633,9 @@
       <c r="I185" s="1">
         <v>28783</v>
       </c>
-      <c r="J185" s="1"/>
+      <c r="J185" s="1">
+        <v>28784</v>
+      </c>
     </row>
     <row r="186" spans="1:10">
       <c r="A186">
@@ -8611,7 +8665,9 @@
       <c r="I186" s="1">
         <v>20272</v>
       </c>
-      <c r="J186" s="1"/>
+      <c r="J186" s="1">
+        <v>20372</v>
+      </c>
     </row>
     <row r="187" spans="1:10">
       <c r="A187">
@@ -8641,7 +8697,9 @@
       <c r="I187" s="1">
         <v>20272</v>
       </c>
-      <c r="J187" s="1"/>
+      <c r="J187" s="1">
+        <v>20372</v>
+      </c>
     </row>
     <row r="188" spans="1:10">
       <c r="A188">
@@ -8671,7 +8729,9 @@
       <c r="I188" s="1">
         <v>20272</v>
       </c>
-      <c r="J188" s="1"/>
+      <c r="J188" s="1">
+        <v>20372</v>
+      </c>
     </row>
     <row r="189" spans="1:10">
       <c r="A189">
@@ -8701,7 +8761,9 @@
       <c r="I189" s="1">
         <v>28783</v>
       </c>
-      <c r="J189" s="1"/>
+      <c r="J189" s="1">
+        <v>28784</v>
+      </c>
     </row>
     <row r="190" spans="1:10">
       <c r="A190">
@@ -8731,7 +8793,9 @@
       <c r="I190" s="1">
         <v>20272</v>
       </c>
-      <c r="J190" s="1"/>
+      <c r="J190" s="1">
+        <v>20372</v>
+      </c>
     </row>
     <row r="191" spans="1:10">
       <c r="A191">
@@ -8761,7 +8825,9 @@
       <c r="I191" s="1">
         <v>20272</v>
       </c>
-      <c r="J191" s="1"/>
+      <c r="J191" s="1">
+        <v>20372</v>
+      </c>
     </row>
     <row r="192" spans="1:10">
       <c r="A192">
@@ -8791,37 +8857,41 @@
       <c r="I192" s="1">
         <v>20272</v>
       </c>
-      <c r="J192" s="1"/>
-    </row>
-    <row r="193" spans="1:10">
-      <c r="A193">
+      <c r="J192" s="1">
+        <v>20372</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" s="6" customFormat="1">
+      <c r="A193" s="6">
         <v>5359</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B193" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="C193" s="1" t="s">
+      <c r="C193" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="D193" s="1" t="s">
+      <c r="D193" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="E193" s="1" t="s">
+      <c r="E193" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="F193" s="1" t="s">
+      <c r="F193" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="G193" s="1">
-        <v>0</v>
-      </c>
-      <c r="H193" s="1">
-        <v>0</v>
-      </c>
-      <c r="I193" s="1">
+      <c r="G193" s="7">
+        <v>0</v>
+      </c>
+      <c r="H193" s="7">
+        <v>0</v>
+      </c>
+      <c r="I193" s="7">
         <v>28673</v>
       </c>
-      <c r="J193" s="1"/>
+      <c r="J193" s="7" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="194" spans="1:10">
       <c r="A194">
@@ -8851,7 +8921,9 @@
       <c r="I194" s="1">
         <v>20272</v>
       </c>
-      <c r="J194" s="1"/>
+      <c r="J194" s="1">
+        <v>20372</v>
+      </c>
     </row>
     <row r="195" spans="1:10">
       <c r="A195">
@@ -8881,7 +8953,9 @@
       <c r="I195" s="1">
         <v>28783</v>
       </c>
-      <c r="J195" s="1"/>
+      <c r="J195" s="1">
+        <v>28784</v>
+      </c>
     </row>
     <row r="196" spans="1:10">
       <c r="A196">
@@ -8911,7 +8985,9 @@
       <c r="I196" s="1">
         <v>29668</v>
       </c>
-      <c r="J196" s="1"/>
+      <c r="J196" s="1">
+        <v>29663</v>
+      </c>
     </row>
     <row r="197" spans="1:10">
       <c r="A197">
@@ -8973,37 +9049,41 @@
       <c r="I198" s="1">
         <v>21169</v>
       </c>
-      <c r="J198" s="1"/>
-    </row>
-    <row r="199" spans="1:10">
-      <c r="A199">
+      <c r="J198" s="1">
+        <v>21167</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" s="6" customFormat="1">
+      <c r="A199" s="6">
         <v>5460</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B199" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="C199" s="1" t="s">
+      <c r="C199" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="D199" s="1" t="s">
+      <c r="D199" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="E199" s="1" t="s">
+      <c r="E199" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="F199" s="1" t="s">
+      <c r="F199" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="G199" s="1">
-        <v>0</v>
-      </c>
-      <c r="H199" s="1">
-        <v>0</v>
-      </c>
-      <c r="I199" s="1">
+      <c r="G199" s="7">
+        <v>0</v>
+      </c>
+      <c r="H199" s="7">
+        <v>0</v>
+      </c>
+      <c r="I199" s="7">
         <v>28637</v>
       </c>
-      <c r="J199" s="1"/>
+      <c r="J199" s="7" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="200" spans="1:10">
       <c r="A200">
@@ -9033,7 +9113,9 @@
       <c r="I200" s="1">
         <v>26455</v>
       </c>
-      <c r="J200" s="1"/>
+      <c r="J200" s="1">
+        <v>26152</v>
+      </c>
     </row>
     <row r="201" spans="1:10">
       <c r="A201">
@@ -9095,7 +9177,9 @@
       <c r="I202" s="1">
         <v>20999</v>
       </c>
-      <c r="J202" s="1"/>
+      <c r="J202" s="1">
+        <v>20998</v>
+      </c>
     </row>
     <row r="203" spans="1:10">
       <c r="A203">
@@ -9125,7 +9209,9 @@
       <c r="I203" s="1">
         <v>22277</v>
       </c>
-      <c r="J203" s="1"/>
+      <c r="J203" s="1">
+        <v>22272</v>
+      </c>
     </row>
     <row r="204" spans="1:10">
       <c r="A204">
@@ -9155,7 +9241,9 @@
       <c r="I204" s="1">
         <v>28783</v>
       </c>
-      <c r="J204" s="1"/>
+      <c r="J204" s="1">
+        <v>28784</v>
+      </c>
     </row>
     <row r="205" spans="1:10">
       <c r="A205">
@@ -9185,7 +9273,9 @@
       <c r="I205" s="1">
         <v>29358</v>
       </c>
-      <c r="J205" s="1"/>
+      <c r="J205" s="1">
+        <v>29352</v>
+      </c>
     </row>
     <row r="206" spans="1:10">
       <c r="A206">
@@ -9215,7 +9305,9 @@
       <c r="I206" s="1">
         <v>59460</v>
       </c>
-      <c r="J206" s="1"/>
+      <c r="J206" s="1">
+        <v>59462</v>
+      </c>
     </row>
     <row r="207" spans="1:10">
       <c r="A207">
@@ -9277,7 +9369,9 @@
       <c r="I208" s="1">
         <v>57523</v>
       </c>
-      <c r="J208" s="1"/>
+      <c r="J208" s="1">
+        <v>57253</v>
+      </c>
     </row>
     <row r="209" spans="1:10">
       <c r="A209">
@@ -9339,7 +9433,9 @@
       <c r="I210" s="1">
         <v>41386</v>
       </c>
-      <c r="J210" s="1"/>
+      <c r="J210" s="1">
+        <v>41384</v>
+      </c>
     </row>
     <row r="211" spans="1:10">
       <c r="A211">
@@ -9369,7 +9465,9 @@
       <c r="I211" s="1">
         <v>28783</v>
       </c>
-      <c r="J211" s="1"/>
+      <c r="J211" s="1">
+        <v>28784</v>
+      </c>
     </row>
     <row r="212" spans="1:10">
       <c r="A212">
@@ -9399,7 +9497,9 @@
       <c r="I212" s="1">
         <v>28783</v>
       </c>
-      <c r="J212" s="1"/>
+      <c r="J212" s="1">
+        <v>28784</v>
+      </c>
     </row>
     <row r="213" spans="1:10">
       <c r="A213">
@@ -9429,7 +9529,9 @@
       <c r="I213" s="1">
         <v>20272</v>
       </c>
-      <c r="J213" s="1"/>
+      <c r="J213" s="1">
+        <v>20372</v>
+      </c>
     </row>
     <row r="214" spans="1:10">
       <c r="A214">
@@ -9459,7 +9561,9 @@
       <c r="I214" s="1">
         <v>28783</v>
       </c>
-      <c r="J214" s="1"/>
+      <c r="J214" s="1">
+        <v>28784</v>
+      </c>
     </row>
     <row r="215" spans="1:10">
       <c r="A215">
@@ -9553,7 +9657,9 @@
       <c r="I217" s="1">
         <v>20272</v>
       </c>
-      <c r="J217" s="1"/>
+      <c r="J217" s="1">
+        <v>20372</v>
+      </c>
     </row>
     <row r="218" spans="1:10">
       <c r="A218">
@@ -9583,7 +9689,9 @@
       <c r="I218" s="1">
         <v>28783</v>
       </c>
-      <c r="J218" s="1"/>
+      <c r="J218" s="1">
+        <v>28784</v>
+      </c>
     </row>
     <row r="219" spans="1:10">
       <c r="A219">
@@ -9613,7 +9721,9 @@
       <c r="I219" s="1">
         <v>20272</v>
       </c>
-      <c r="J219" s="1"/>
+      <c r="J219" s="1">
+        <v>20372</v>
+      </c>
     </row>
     <row r="220" spans="1:10">
       <c r="A220">
@@ -9643,7 +9753,9 @@
       <c r="I220" s="1">
         <v>28783</v>
       </c>
-      <c r="J220" s="1"/>
+      <c r="J220" s="1">
+        <v>28784</v>
+      </c>
     </row>
     <row r="221" spans="1:10">
       <c r="A221">
@@ -9737,7 +9849,9 @@
       <c r="I223" s="1">
         <v>28783</v>
       </c>
-      <c r="J223" s="1"/>
+      <c r="J223" s="1">
+        <v>28784</v>
+      </c>
     </row>
     <row r="224" spans="1:10">
       <c r="A224">
@@ -9767,7 +9881,9 @@
       <c r="I224" s="1">
         <v>80363</v>
       </c>
-      <c r="J224" s="1"/>
+      <c r="J224" s="1">
+        <v>80361</v>
+      </c>
     </row>
     <row r="225" spans="1:10">
       <c r="A225">
@@ -9829,7 +9945,9 @@
       <c r="I226" s="1">
         <v>17750</v>
       </c>
-      <c r="J226" s="1"/>
+      <c r="J226" s="1">
+        <v>17530</v>
+      </c>
     </row>
     <row r="227" spans="1:10">
       <c r="A227">
@@ -9955,7 +10073,9 @@
       <c r="I230" s="1">
         <v>17352</v>
       </c>
-      <c r="J230" s="1"/>
+      <c r="J230" s="1">
+        <v>17350</v>
+      </c>
     </row>
     <row r="231" spans="1:10">
       <c r="A231">
@@ -10017,7 +10137,9 @@
       <c r="I232" s="1">
         <v>20272</v>
       </c>
-      <c r="J232" s="1"/>
+      <c r="J232" s="1">
+        <v>20372</v>
+      </c>
     </row>
     <row r="233" spans="1:10">
       <c r="A233">
@@ -10047,7 +10169,9 @@
       <c r="I233" s="1">
         <v>57523</v>
       </c>
-      <c r="J233" s="1"/>
+      <c r="J233" s="1">
+        <v>57253</v>
+      </c>
     </row>
     <row r="234" spans="1:10">
       <c r="A234">
@@ -10141,7 +10265,9 @@
       <c r="I236" s="1">
         <v>28296</v>
       </c>
-      <c r="J236" s="1"/>
+      <c r="J236" s="1">
+        <v>28293</v>
+      </c>
     </row>
     <row r="237" spans="1:10">
       <c r="A237">
@@ -10203,7 +10329,9 @@
       <c r="I238" s="1">
         <v>28783</v>
       </c>
-      <c r="J238" s="1"/>
+      <c r="J238" s="1">
+        <v>28784</v>
+      </c>
     </row>
     <row r="239" spans="1:10">
       <c r="A239">
@@ -10233,7 +10361,9 @@
       <c r="I239" s="1">
         <v>20272</v>
       </c>
-      <c r="J239" s="1"/>
+      <c r="J239" s="1">
+        <v>20372</v>
+      </c>
     </row>
     <row r="240" spans="1:10">
       <c r="A240">
@@ -10295,7 +10425,9 @@
       <c r="I241" s="1">
         <v>30761</v>
       </c>
-      <c r="J241" s="1"/>
+      <c r="J241" s="1">
+        <v>30961</v>
+      </c>
     </row>
     <row r="242" spans="1:10">
       <c r="A242">
@@ -10357,7 +10489,9 @@
       <c r="I243" s="1">
         <v>20985</v>
       </c>
-      <c r="J243" s="1"/>
+      <c r="J243" s="1">
+        <v>20986</v>
+      </c>
     </row>
     <row r="244" spans="1:10">
       <c r="A244">
@@ -10419,7 +10553,9 @@
       <c r="I245" s="1">
         <v>61131</v>
       </c>
-      <c r="J245" s="1"/>
+      <c r="J245" s="1">
+        <v>61151</v>
+      </c>
     </row>
     <row r="246" spans="1:10">
       <c r="A246">
@@ -10449,7 +10585,9 @@
       <c r="I246" s="1">
         <v>16611</v>
       </c>
-      <c r="J246" s="1"/>
+      <c r="J246" s="1">
+        <v>16610</v>
+      </c>
     </row>
     <row r="247" spans="1:10">
       <c r="A247">
@@ -10479,7 +10617,9 @@
       <c r="I247" s="1">
         <v>19110</v>
       </c>
-      <c r="J247" s="1"/>
+      <c r="J247" s="1">
+        <v>15125</v>
+      </c>
     </row>
     <row r="248" spans="1:10">
       <c r="A248">
@@ -10605,7 +10745,9 @@
       <c r="I251" s="1">
         <v>17450</v>
       </c>
-      <c r="J251" s="1"/>
+      <c r="J251" s="1">
+        <v>17540</v>
+      </c>
     </row>
     <row r="252" spans="1:10">
       <c r="A252">
@@ -10635,7 +10777,9 @@
       <c r="I252" s="1">
         <v>17450</v>
       </c>
-      <c r="J252" s="1"/>
+      <c r="J252" s="1">
+        <v>17540</v>
+      </c>
     </row>
     <row r="253" spans="1:10">
       <c r="A253">
@@ -10761,7 +10905,9 @@
       <c r="I256" s="1">
         <v>17450</v>
       </c>
-      <c r="J256" s="1"/>
+      <c r="J256" s="1">
+        <v>17540</v>
+      </c>
     </row>
     <row r="257" spans="1:10">
       <c r="A257">
@@ -10791,7 +10937,9 @@
       <c r="I257" s="1">
         <v>21276</v>
       </c>
-      <c r="J257" s="1"/>
+      <c r="J257" s="1">
+        <v>21274</v>
+      </c>
     </row>
     <row r="258" spans="1:10">
       <c r="A258">
@@ -10885,7 +11033,9 @@
       <c r="I260" s="1">
         <v>28296</v>
       </c>
-      <c r="J260" s="1"/>
+      <c r="J260" s="1">
+        <v>28293</v>
+      </c>
     </row>
     <row r="261" spans="1:10">
       <c r="A261">
@@ -10915,7 +11065,9 @@
       <c r="I261" s="1">
         <v>28296</v>
       </c>
-      <c r="J261" s="1"/>
+      <c r="J261" s="1">
+        <v>28293</v>
+      </c>
     </row>
     <row r="262" spans="1:10">
       <c r="A262">
@@ -11105,7 +11257,9 @@
       <c r="I267" s="1">
         <v>21160</v>
       </c>
-      <c r="J267" s="1"/>
+      <c r="J267" s="1">
+        <v>21162</v>
+      </c>
     </row>
     <row r="268" spans="1:10">
       <c r="A268">
@@ -11199,7 +11353,9 @@
       <c r="I270" s="1">
         <v>42421</v>
       </c>
-      <c r="J270" s="1"/>
+      <c r="J270" s="1">
+        <v>42161</v>
+      </c>
     </row>
     <row r="271" spans="1:10">
       <c r="A271">
@@ -11325,7 +11481,9 @@
       <c r="I274" s="1">
         <v>22730</v>
       </c>
-      <c r="J274" s="1"/>
+      <c r="J274" s="1">
+        <v>22733</v>
+      </c>
     </row>
     <row r="275" spans="1:10">
       <c r="A275">
@@ -11355,7 +11513,9 @@
       <c r="I275" s="1">
         <v>34694</v>
       </c>
-      <c r="J275" s="1"/>
+      <c r="J275" s="1">
+        <v>34684</v>
+      </c>
     </row>
     <row r="276" spans="1:10">
       <c r="A276">
@@ -11385,7 +11545,9 @@
       <c r="I276" s="1">
         <v>20776</v>
       </c>
-      <c r="J276" s="1"/>
+      <c r="J276" s="1">
+        <v>20773</v>
+      </c>
     </row>
     <row r="277" spans="1:10">
       <c r="A277">
@@ -11447,7 +11609,9 @@
       <c r="I278" s="1">
         <v>28783</v>
       </c>
-      <c r="J278" s="1"/>
+      <c r="J278" s="1">
+        <v>28784</v>
+      </c>
     </row>
     <row r="279" spans="1:10">
       <c r="A279">
@@ -11509,7 +11673,9 @@
       <c r="I280" s="1">
         <v>21277</v>
       </c>
-      <c r="J280" s="1"/>
+      <c r="J280" s="1">
+        <v>21273</v>
+      </c>
     </row>
     <row r="281" spans="1:10">
       <c r="A281">
@@ -11699,7 +11865,9 @@
       <c r="I286" s="1">
         <v>37317</v>
       </c>
-      <c r="J286" s="1"/>
+      <c r="J286" s="1">
+        <v>37311</v>
+      </c>
     </row>
     <row r="287" spans="1:10">
       <c r="A287">
@@ -11921,7 +12089,9 @@
       <c r="I293" s="1">
         <v>35352</v>
       </c>
-      <c r="J293" s="1"/>
+      <c r="J293" s="1">
+        <v>35353</v>
+      </c>
     </row>
     <row r="294" spans="1:10">
       <c r="A294">

</xml_diff>